<commit_message>
Troubleshooting (reservoir levels, non-integer min up/down times) Generalized the standard test case with HDAM Added initial state in the power plant inputs Improved model ergonomy
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="155">
   <si>
     <t>Default value</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Simulations/simulation_test</t>
   </si>
   <si>
-    <t>Dummy configuration file for testing purposes. The data used for the simulation is the dutch data. The simulated period is only 10 days.</t>
-  </si>
-  <si>
     <t>Price of Lignite</t>
   </si>
   <si>
@@ -469,6 +466,21 @@
   </si>
   <si>
     <t>Database/DummyData/Outages.csv</t>
+  </si>
+  <si>
+    <t>CPLEX path</t>
+  </si>
+  <si>
+    <t>Dummy configuration file for testing purposes. Two fictitious zones (Z1 and Z2) are simulated. The simulated period is only 10 days.</t>
+  </si>
+  <si>
+    <t>Database/DummyData/ScaledInflows.csv</t>
+  </si>
+  <si>
+    <t>Database/DummyData/ReservoirLevels.csv</t>
+  </si>
+  <si>
+    <t>Heat Demand</t>
   </si>
 </sst>
 </file>
@@ -954,8 +966,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1032,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -1108,7 +1120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>90</v>
       </c>
@@ -1119,12 +1131,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" ht="0.75" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
@@ -1278,7 +1301,7 @@
         <v>37</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>94</v>
@@ -1293,7 +1316,7 @@
         <v>37</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>94</v>
@@ -1310,7 +1333,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>94</v>
@@ -1327,7 +1350,7 @@
         <v>37</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>94</v>
@@ -1362,7 +1385,7 @@
         <v>37</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>94</v>
@@ -1379,7 +1402,7 @@
         <v>37</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D68" s="22" t="s">
         <v>94</v>
@@ -1395,7 +1418,9 @@
       <c r="B69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="24"/>
+      <c r="C69" s="24" t="s">
+        <v>152</v>
+      </c>
       <c r="D69" s="22" t="s">
         <v>94</v>
       </c>
@@ -1527,14 +1552,16 @@
       <c r="B76" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="24"/>
+      <c r="C76" s="24" t="s">
+        <v>153</v>
+      </c>
       <c r="D76" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>37</v>
@@ -1550,9 +1577,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>37</v>
@@ -1570,12 +1597,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="24"/>
+      <c r="D79" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:6" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="C85" s="18"/>
@@ -1607,7 +1645,7 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="29"/>
       <c r="B89" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C89" s="4" t="b">
         <v>1</v>
@@ -1688,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F94" s="5" t="b">
         <v>1</v>
@@ -2030,7 +2068,7 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B4:H4"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31:D31">
       <formula1>1</formula1>
@@ -2049,6 +2087,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
simplified/corrected up down time constraints in the rolling horizon
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -984,8 +984,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,7 +1924,7 @@
         <v>79</v>
       </c>
       <c r="C112" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
efficiencies and COP are now time-dependent
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD33D53-E0E9-4688-B490-24F48A859807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F88152-4C01-4FA9-9FC6-CD8557AC8625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="211">
   <si>
     <t>Default value</t>
   </si>
@@ -605,15 +605,9 @@
     <t>This section provides the paths or default values for the additional Dispa-SET parameters</t>
   </si>
   <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>The path is a relative path,with reference to the current working directory, or an absolute path</t>
   </si>
   <si>
-    <t>Database/Temperatures/temps_2016.csv</t>
-  </si>
-  <si>
     <t>Additional Input Data (to be merged above when refactoring the config file)</t>
   </si>
   <si>
@@ -666,6 +660,12 @@
   </si>
   <si>
     <t>Z2</t>
+  </si>
+  <si>
+    <t>Temperatures</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Temperatures.csv</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1436,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
@@ -1509,7 +1509,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
@@ -1719,11 +1719,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="C51" s="1"/>
     </row>
@@ -1826,7 +1826,7 @@
         <v>37</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>92</v>
@@ -1841,7 +1841,7 @@
         <v>37</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>92</v>
@@ -1858,7 +1858,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>92</v>
@@ -1875,7 +1875,7 @@
         <v>37</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>92</v>
@@ -1885,7 +1885,10 @@
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="35"/>
+      <c r="B66" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" s="19"/>
       <c r="D66" s="18" t="s">
         <v>92</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>37</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>92</v>
@@ -1924,7 +1927,7 @@
         <v>37</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>92</v>
@@ -1941,7 +1944,7 @@
         <v>37</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>92</v>
@@ -1974,7 +1977,7 @@
         <v>37</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>92</v>
@@ -1994,7 +1997,7 @@
         <v>37</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>92</v>
@@ -2017,7 +2020,7 @@
         <v>37</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>92</v>
@@ -2037,7 +2040,7 @@
         <v>37</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>92</v>
@@ -2075,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>92</v>
@@ -2107,7 +2110,7 @@
         <v>37</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>92</v>
@@ -2127,7 +2130,7 @@
         <v>37</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>92</v>
@@ -2155,7 +2158,10 @@
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C81" s="35"/>
+      <c r="B81" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81" s="19"/>
       <c r="D81" s="18" t="s">
         <v>92</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F87" s="4" t="b">
         <v>1</v>
@@ -2270,7 +2276,7 @@
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C88" s="4" t="b">
         <v>1</v>
@@ -2935,7 +2941,7 @@
     </row>
     <row r="156" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B156" s="37"/>
       <c r="C156" s="38"/>
@@ -2947,13 +2953,13 @@
     </row>
     <row r="157" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="B157" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C157" s="19" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="D157" s="18" t="s">
         <v>92</v>
@@ -2981,7 +2987,7 @@
         <v>92</v>
       </c>
       <c r="H159" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
pre-processing with variable time step
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F88152-4C01-4FA9-9FC6-CD8557AC8625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D735B0D0-DC7B-4EC4-8656-CF3DFC730D03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="214">
   <si>
     <t>Default value</t>
   </si>
@@ -666,6 +666,15 @@
   </si>
   <si>
     <t>tests/dummy_data/Temperatures.csv</t>
+  </si>
+  <si>
+    <t>Time step in the data</t>
+  </si>
+  <si>
+    <t>Simulation time step</t>
+  </si>
+  <si>
+    <t>Number of hours</t>
   </si>
 </sst>
 </file>
@@ -961,6 +970,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,9 +984,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1369,8 +1378,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,16 +1396,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1411,15 +1420,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1435,15 +1444,15 @@
       <c r="A6" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -1652,16 +1661,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:8" ht="10.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
         <v>171</v>
@@ -2272,7 +2301,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="46" t="s">
+      <c r="A88" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -2295,7 +2324,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="46"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="6" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2345,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="46"/>
+      <c r="A90" s="47"/>
       <c r="B90" s="6" t="s">
         <v>156</v>
       </c>
@@ -2337,7 +2366,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="46"/>
+      <c r="A91" s="47"/>
       <c r="B91" s="6" t="s">
         <v>138</v>
       </c>
@@ -2358,7 +2387,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="46"/>
+      <c r="A92" s="47"/>
       <c r="B92" s="6" t="s">
         <v>5</v>
       </c>
@@ -2379,7 +2408,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="46"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="6" t="s">
         <v>159</v>
       </c>
@@ -2400,7 +2429,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="46"/>
+      <c r="A94" s="47"/>
       <c r="B94" s="6" t="s">
         <v>31</v>
       </c>
@@ -2421,7 +2450,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="46"/>
+      <c r="A95" s="47"/>
       <c r="B95" s="6" t="s">
         <v>16</v>
       </c>
@@ -2442,7 +2471,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="46"/>
+      <c r="A96" s="47"/>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
@@ -2463,7 +2492,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="46"/>
+      <c r="A97" s="47"/>
       <c r="B97" s="6" t="s">
         <v>8</v>
       </c>
@@ -2484,7 +2513,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="46"/>
+      <c r="A98" s="47"/>
       <c r="B98" s="6" t="s">
         <v>7</v>
       </c>
@@ -2505,7 +2534,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="46"/>
+      <c r="A99" s="47"/>
       <c r="B99" s="6" t="s">
         <v>9</v>
       </c>
@@ -2526,7 +2555,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="46"/>
+      <c r="A100" s="47"/>
       <c r="B100" s="6" t="s">
         <v>11</v>
       </c>
@@ -2547,7 +2576,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="46"/>
+      <c r="A101" s="47"/>
       <c r="B101" s="6" t="s">
         <v>12</v>
       </c>
@@ -2568,7 +2597,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="46"/>
+      <c r="A102" s="47"/>
       <c r="B102" s="6" t="s">
         <v>28</v>
       </c>
@@ -2649,7 +2678,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="s">
+      <c r="A106" s="50" t="s">
         <v>177</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -2672,7 +2701,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="49"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="6" t="s">
         <v>165</v>
       </c>
@@ -3039,7 +3068,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="24">
+  <dataValidations xWindow="547" yWindow="733" count="26">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3076,6 +3105,14 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F57" xr:uid="{C22C312A-4C0D-465E-AA40-04829D4E1DD5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F58" xr:uid="{70E3A2FC-178F-4589-82CF-31382B011A9B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C157" xr:uid="{DCD0DDF5-CAA3-4B00-8005-5B7C31C37DA9}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time step of the data" prompt="This is the time resolution of the time series in the input data. Set to 0.25 for 15min data" sqref="C35" xr:uid="{BFA86061-3576-41E2-AD45-85BBFB43E871}">
+      <formula1>1</formula1>
+      <formula2>365</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Simulation time step" prompt="This is the time step with which to perform the optimization. If different from the time step in the data, all time series will be resampled._x000a_" sqref="C36" xr:uid="{42C50E91-C839-4C42-886E-CA783EE0C609}">
+      <formula1>0</formula1>
+      <formula2>365</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
many corrections to get everything working again
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F51CC6B-FDB5-4E33-85AB-6CD5F8733936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8742B17B-05F2-4BBA-AAC6-8B14D9E3E2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="218">
   <si>
     <t>Default value</t>
   </si>
@@ -663,6 +663,30 @@
   </si>
   <si>
     <t>Value of lost load  in EUR/MWh</t>
+  </si>
+  <si>
+    <t>Time step in the data</t>
+  </si>
+  <si>
+    <t>Simulation time step</t>
+  </si>
+  <si>
+    <t>Number of hours</t>
+  </si>
+  <si>
+    <t>Share of quick start</t>
+  </si>
+  <si>
+    <t>Share of the 2U reserve that can be covered by quick start units</t>
+  </si>
+  <si>
+    <t>Demand flexibility</t>
+  </si>
+  <si>
+    <t>Number of equivalent storage hours for the flexibile demand</t>
+  </si>
+  <si>
+    <t>End of the Config file. This must be line number 325!</t>
   </si>
 </sst>
 </file>
@@ -977,21 +1001,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -1380,8 +1390,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="A326" sqref="A326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,19 +1742,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:8" ht="10.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:8" ht="6.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
@@ -2283,17 +2313,38 @@
       <c r="A161" s="25"/>
       <c r="C161" s="27"/>
     </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25"/>
       <c r="C162" s="27"/>
     </row>
-    <row r="163" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="25"/>
-      <c r="C163" s="27"/>
-    </row>
-    <row r="164" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="25"/>
-      <c r="C164" s="27"/>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C163" s="1"/>
+      <c r="E163" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F163" s="5">
+        <v>4</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E164" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F164" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
@@ -2638,7 +2689,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2652,10 +2703,6 @@
       <c r="H207" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="25"/>
-      <c r="C208" s="27"/>
     </row>
     <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="25"/>
@@ -2693,11 +2740,11 @@
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
@@ -2713,7 +2760,7 @@
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
@@ -3543,7 +3590,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3556,22 +3608,22 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C226:D247 F226:G247 C79 C306:C320 C35:C36">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="26">
+  <dataValidations xWindow="547" yWindow="733" count="28">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3593,11 +3645,11 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C60" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C60 C62" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>0</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C59" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C59 C61" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
@@ -3610,6 +3662,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C136" xr:uid="{DCD0DDF5-CAA3-4B00-8005-5B7C31C37DA9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand input file" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="C126" xr:uid="{C0A91F47-4A7A-4D7C-8BF7-42344234CEB1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand default value" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="F126" xr:uid="{0207F56E-8010-40B0-B53E-04E2603C9864}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F164" xr:uid="{9C9B8F4F-043F-41E7-8848-A40DCB72B3F5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F163" xr:uid="{C47BA5BE-2C24-4654-BEF9-EA5B433BE488}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bug fixes + activated flexible load in the test config file
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8742B17B-05F2-4BBA-AAC6-8B14D9E3E2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95863F92-577D-4362-8AF6-164CE69B66FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="219">
   <si>
     <t>Default value</t>
   </si>
@@ -687,6 +687,9 @@
   </si>
   <si>
     <t>End of the Config file. This must be line number 325!</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/ScaledInflows.csv</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1393,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="A326" sqref="A326"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="5">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H126" s="11"/>
     </row>
@@ -2161,7 +2164,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>89</v>
@@ -2698,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>150</v>

</xml_diff>

<commit_message>
Added pre-processing for PriceTransmission
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95863F92-577D-4362-8AF6-164CE69B66FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929BEA10-1DB6-4393-9303-93E4A759BA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="221">
   <si>
     <t>Default value</t>
   </si>
@@ -690,6 +690,12 @@
   </si>
   <si>
     <t>tests/dummy_data/ScaledInflows.csv</t>
+  </si>
+  <si>
+    <t>Price of Transmission</t>
+  </si>
+  <si>
+    <t>Price related to the usage of tranmission lines (in €/MWh)</t>
   </si>
 </sst>
 </file>
@@ -1393,8 +1399,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,7 +2407,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2422,43 +2428,60 @@
         <v>178</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="25"/>
-      <c r="C170" s="27"/>
-    </row>
-    <row r="171" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B170" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C170" s="19"/>
+      <c r="D170" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E170" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F170" s="5">
+        <v>0</v>
+      </c>
+      <c r="H170" s="26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25"/>
       <c r="C171" s="27"/>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
@@ -3626,7 +3649,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="28">
+  <dataValidations xWindow="547" yWindow="733" count="31">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3667,6 +3690,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand default value" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="F126" xr:uid="{0207F56E-8010-40B0-B53E-04E2603C9864}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F164" xr:uid="{9C9B8F4F-043F-41E7-8848-A40DCB72B3F5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F163" xr:uid="{C47BA5BE-2C24-4654-BEF9-EA5B433BE488}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Exogenous reserves should now be OK. Also included in test config file.
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929BEA10-1DB6-4393-9303-93E4A759BA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E88C6C-754F-462B-A312-BC82A51E328D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
   <si>
     <t>Default value</t>
   </si>
@@ -696,6 +696,15 @@
   </si>
   <si>
     <t>Price related to the usage of tranmission lines (in €/MWh)</t>
+  </si>
+  <si>
+    <t>Reserves Down</t>
+  </si>
+  <si>
+    <t>Reserves Up</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Reserve2U.csv</t>
   </si>
 </sst>
 </file>
@@ -1399,8 +1408,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A183" sqref="A183"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,17 +2323,29 @@
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="25"/>
-      <c r="C161" s="27"/>
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="B161" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C161" s="19" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="25"/>
-      <c r="C162" s="27"/>
+      <c r="A162" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="B162" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C162" s="19"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
@@ -3649,7 +3670,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="31">
+  <dataValidations xWindow="547" yWindow="733" count="33">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3693,6 +3714,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first pre-processing attemps with H2 demand
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E88C6C-754F-462B-A312-BC82A51E328D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA9B92E-514F-4561-BD7F-6FC43A26CFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="227">
   <si>
     <t>Default value</t>
   </si>
@@ -705,6 +705,15 @@
   </si>
   <si>
     <t>tests/dummy_data/Reserve2U.csv</t>
+  </si>
+  <si>
+    <t>Price of Unserved H2</t>
+  </si>
+  <si>
+    <t>H2 Demand</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/H2Demand.csv</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1417,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,9 +2240,19 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="25"/>
-      <c r="C137" s="27"/>
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B137" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C137" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
@@ -2287,11 +2306,11 @@
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
@@ -2449,7 +2468,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>219</v>
       </c>
@@ -2470,43 +2489,57 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="25"/>
-      <c r="C171" s="27"/>
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B171" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C171" s="19"/>
+      <c r="D171" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E171" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F171" s="5">
+        <v>75</v>
+      </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
@@ -3670,7 +3703,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="33">
+  <dataValidations xWindow="547" yWindow="733" count="35">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3681,14 +3714,14 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C37" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F169" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F171" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
@@ -3700,7 +3733,7 @@
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169:F170" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F206" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F207" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
@@ -3716,6 +3749,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{F5C6CB55-A203-47FE-96B0-DC9C451014C9}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit all database for paper
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA9B92E-514F-4561-BD7F-6FC43A26CFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCF4DD6-197D-4A82-A688-9D6542859135}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1094,7 +1094,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1417,24 +1417,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="G226" sqref="G226"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.26953125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>206</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1456,8 +1456,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
         <v>57</v>
@@ -1469,7 +1469,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1479,7 +1479,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -1502,7 +1502,7 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
@@ -1511,7 +1511,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -1520,7 +1520,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1529,7 +1529,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -1538,7 +1538,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -1547,7 +1547,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -1556,7 +1556,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
     </row>
-    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1565,7 +1565,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="35" t="s">
         <v>180</v>
       </c>
@@ -1577,39 +1577,39 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="29"/>
     </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="30"/>
     </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="35" t="s">
         <v>170</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>131</v>
       </c>
@@ -1687,24 +1687,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="35" t="s">
         <v>169</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>48</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>210</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
@@ -1788,22 +1788,22 @@
         <v>212</v>
       </c>
       <c r="C62" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="35" t="s">
         <v>167</v>
       </c>
@@ -1815,10 +1815,10 @@
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -1860,76 +1860,76 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="35" t="s">
         <v>174</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>140</v>
       </c>
@@ -1949,13 +1949,13 @@
         <v>60</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>163</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>177</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="32" t="s">
         <v>175</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="32" t="s">
         <v>176</v>
       </c>
@@ -2008,30 +2008,30 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="35" t="s">
         <v>168</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="36"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>204</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>37</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>41</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>49</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>90</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>128</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>201</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>225</v>
       </c>
@@ -2254,99 +2254,99 @@
         <v>89</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="25"/>
       <c r="C138" s="27"/>
     </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="25"/>
       <c r="C139" s="27"/>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="25"/>
       <c r="C140" s="27"/>
     </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="25"/>
       <c r="C141" s="27"/>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="25"/>
       <c r="C142" s="27"/>
     </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
         <v>222</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="25" t="s">
         <v>221</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>215</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>213</v>
       </c>
@@ -2395,11 +2395,11 @@
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="25"/>
       <c r="C165" s="27"/>
     </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="35" t="s">
         <v>203</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="36"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>124</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
         <v>219</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>224</v>
       </c>
@@ -2507,43 +2507,43 @@
         <v>75</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>122</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
         <v>91</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
         <v>63</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
         <v>123</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
         <v>129</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>130</v>
       </c>
@@ -2680,66 +2680,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="25"/>
       <c r="C188" s="27"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="25"/>
       <c r="C192" s="27"/>
     </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="25"/>
       <c r="C193" s="27"/>
     </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
     </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="25"/>
       <c r="C195" s="27"/>
     </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="25"/>
       <c r="C196" s="27"/>
     </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="25"/>
       <c r="C197" s="27"/>
     </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="25"/>
       <c r="C198" s="27"/>
     </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="25"/>
       <c r="C199" s="27"/>
     </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="25"/>
       <c r="C200" s="27"/>
     </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="25"/>
       <c r="C201" s="27"/>
     </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="25"/>
       <c r="C202" s="27"/>
     </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="25"/>
       <c r="C203" s="27"/>
     </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>147</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>145</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2784,71 +2784,71 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="25"/>
       <c r="C209" s="27"/>
     </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="25"/>
       <c r="C210" s="27"/>
     </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="39" t="s">
         <v>171</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="H225" s="40"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>51</v>
       </c>
@@ -2892,10 +2892,10 @@
         <v>1</v>
       </c>
       <c r="G226" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="47" t="s">
         <v>52</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="D227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
         <v>18</v>
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>22</v>
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>152</v>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>134</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>155</v>
@@ -3023,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>31</v>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3065,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3149,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>28</v>
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B244" s="6" t="s">
         <v>20</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="50" t="s">
         <v>173</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>161</v>
@@ -3319,7 +3319,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3339,108 +3339,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A274" s="35" t="s">
         <v>73</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="G274" s="36"/>
       <c r="H274" s="36"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
         <v>74</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
         <v>75</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
         <v>77</v>
       </c>
@@ -3502,35 +3502,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A302" s="9"/>
       <c r="C302" s="14"/>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A304" s="39" t="s">
         <v>172</v>
       </c>
@@ -3542,7 +3542,7 @@
       <c r="G304" s="40"/>
       <c r="H304" s="40"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" s="2" t="s">
         <v>121</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B306" s="22" t="s">
         <v>92</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B307" s="22" t="s">
         <v>93</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B308" s="22" t="s">
         <v>94</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B309" s="22" t="s">
         <v>95</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B310" s="22" t="s">
         <v>96</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B311" s="22" t="s">
         <v>97</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B312" s="22" t="s">
         <v>98</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B313" s="22" t="s">
         <v>99</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B314" s="22" t="s">
         <v>100</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B315" s="22" t="s">
         <v>101</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B316" s="22" t="s">
         <v>102</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B317" s="22" t="s">
         <v>103</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B318" s="22" t="s">
         <v>104</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B319" s="22" t="s">
         <v>105</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B320" s="22" t="s">
         <v>106</v>
       </c>
@@ -3670,12 +3670,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A325" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3826,16 +3826,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3931,12 +3931,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>94</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>97</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>99</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>100</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>104</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>105</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
Water withdrawal and water consumption now included in postprocessing
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\Dispa-SET\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCF4DD6-197D-4A82-A688-9D6542859135}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BE910E-F1B8-434B-B825-2E6DC7FBDFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$78:$C$99</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1094,7 +1094,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1417,24 +1417,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="G226" sqref="G226"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7265625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.26953125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>206</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1456,8 +1456,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
         <v>57</v>
@@ -1469,7 +1469,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1479,7 +1479,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>50</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -1502,7 +1502,7 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
@@ -1511,7 +1511,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -1520,7 +1520,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1529,7 +1529,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -1538,7 +1538,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -1547,7 +1547,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -1556,7 +1556,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
     </row>
-    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1565,7 +1565,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>180</v>
       </c>
@@ -1577,39 +1577,39 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="29"/>
     </row>
-    <row r="17" spans="1:2" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="30"/>
     </row>
-    <row r="18" spans="1:2" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>170</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>131</v>
       </c>
@@ -1687,24 +1687,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>169</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>46</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>48</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>210</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
@@ -1788,22 +1788,22 @@
         <v>212</v>
       </c>
       <c r="C62" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>167</v>
       </c>
@@ -1815,10 +1815,10 @@
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -1860,76 +1860,76 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>174</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>140</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>163</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>177</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
         <v>175</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
         <v>176</v>
       </c>
@@ -2008,30 +2008,30 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
         <v>168</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="36"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>204</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>37</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>41</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>49</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>90</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>128</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>201</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>225</v>
       </c>
@@ -2254,99 +2254,99 @@
         <v>89</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="C138" s="27"/>
     </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25"/>
       <c r="C139" s="27"/>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
       <c r="C140" s="27"/>
     </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
       <c r="C141" s="27"/>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="C142" s="27"/>
     </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="C144" s="27"/>
     </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="25"/>
       <c r="C146" s="27"/>
     </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="C148" s="27"/>
     </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="25"/>
       <c r="C149" s="27"/>
     </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="25"/>
       <c r="C150" s="27"/>
     </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
       <c r="C151" s="27"/>
     </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
       <c r="C152" s="27"/>
     </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="C153" s="27"/>
     </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="C154" s="27"/>
     </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
       <c r="C155" s="27"/>
     </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="C156" s="27"/>
     </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="25"/>
       <c r="C157" s="27"/>
     </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="25"/>
       <c r="C158" s="27"/>
     </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
         <v>222</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
         <v>221</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>215</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>213</v>
       </c>
@@ -2395,11 +2395,11 @@
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
       <c r="C165" s="27"/>
     </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
         <v>203</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="36"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>124</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>138</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>219</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>224</v>
       </c>
@@ -2507,43 +2507,43 @@
         <v>75</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="C172" s="27"/>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="C173" s="27"/>
     </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
     </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="C175" s="27"/>
     </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="C176" s="27"/>
     </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="C177" s="27"/>
     </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="C178" s="27"/>
     </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="C179" s="27"/>
     </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25"/>
       <c r="C180" s="27"/>
     </row>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>122</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>91</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>63</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>123</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>129</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>130</v>
       </c>
@@ -2680,66 +2680,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25"/>
       <c r="C188" s="27"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="25"/>
       <c r="C192" s="27"/>
     </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="25"/>
       <c r="C193" s="27"/>
     </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="25"/>
       <c r="C194" s="27"/>
     </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="25"/>
       <c r="C195" s="27"/>
     </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="25"/>
       <c r="C196" s="27"/>
     </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="25"/>
       <c r="C197" s="27"/>
     </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="25"/>
       <c r="C198" s="27"/>
     </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="25"/>
       <c r="C199" s="27"/>
     </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="25"/>
       <c r="C200" s="27"/>
     </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="25"/>
       <c r="C201" s="27"/>
     </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="25"/>
       <c r="C202" s="27"/>
     </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="25"/>
       <c r="C203" s="27"/>
     </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="25"/>
       <c r="C204" s="27"/>
     </row>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>147</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>145</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>148</v>
       </c>
@@ -2784,71 +2784,71 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="25"/>
       <c r="C209" s="27"/>
     </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="25"/>
       <c r="C210" s="27"/>
     </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="25"/>
       <c r="C211" s="27"/>
     </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="25"/>
       <c r="C212" s="27"/>
     </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="25"/>
       <c r="C213" s="27"/>
     </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="25"/>
       <c r="C214" s="27"/>
     </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="25"/>
       <c r="C215" s="27"/>
     </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="25"/>
       <c r="C216" s="27"/>
     </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="25"/>
       <c r="C217" s="27"/>
     </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="25"/>
       <c r="C218" s="27"/>
     </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="25"/>
       <c r="C219" s="27"/>
     </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="25"/>
       <c r="C220" s="27"/>
     </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="25"/>
       <c r="C221" s="27"/>
     </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="25"/>
       <c r="C222" s="27"/>
     </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="25"/>
       <c r="C223" s="27"/>
     </row>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
         <v>171</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="H225" s="40"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>51</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="47" t="s">
         <v>52</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>22</v>
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>152</v>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>134</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>155</v>
@@ -3023,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>31</v>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3065,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3149,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>28</v>
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
         <v>20</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="50" t="s">
         <v>173</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>161</v>
@@ -3319,7 +3319,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3339,108 +3339,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="35" t="s">
         <v>73</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="G274" s="36"/>
       <c r="H274" s="36"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>74</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>75</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>77</v>
       </c>
@@ -3502,35 +3502,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="9"/>
       <c r="C302" s="14"/>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="39" t="s">
         <v>172</v>
       </c>
@@ -3542,7 +3542,7 @@
       <c r="G304" s="40"/>
       <c r="H304" s="40"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>121</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
         <v>92</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
         <v>93</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
         <v>94</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
         <v>95</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
         <v>96</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
         <v>97</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
         <v>98</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
         <v>99</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
         <v>100</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
         <v>101</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
         <v>102</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
         <v>103</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
         <v>104</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
         <v>105</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
         <v>106</v>
       </c>
@@ -3670,12 +3670,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3826,16 +3826,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3931,12 +3931,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>94</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>97</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>99</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>100</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>104</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>105</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
Basic plotting of net flows on a map (weights included)
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\svn\Dispa-SET_Public\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E88C6C-754F-462B-A312-BC82A51E328D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D279B16-930C-4E3E-A744-8BA323D869BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="225">
   <si>
     <t>Default value</t>
   </si>
@@ -705,6 +705,9 @@
   </si>
   <si>
     <t>tests/dummy_data/Reserve2U.csv</t>
+  </si>
+  <si>
+    <t>Geo Data</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1411,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,9 +2234,14 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="25"/>
-      <c r="C137" s="27"/>
+    <row r="137" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B137" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C137" s="19"/>
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
@@ -3670,7 +3678,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="33">
+  <dataValidations xWindow="547" yWindow="733" count="34">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3716,6 +3724,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Geo spatial location" prompt="Geo spatial locations of selected zones (When not provided built-in function checks internal database)" sqref="C137" xr:uid="{350E1C09-B561-475A-AF77-4C43B79D459A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Output enhancement and minor modifications to reserve equations
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FED7703-0435-4E1C-94F4-9982E8190976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA9A141-710F-4B4C-B2E5-3E3ECCA9EF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>LV</t>
   </si>
   <si>
-    <t>LT</t>
-  </si>
-  <si>
     <t>LU</t>
   </si>
   <si>
@@ -735,6 +732,9 @@
   </si>
   <si>
     <t>tests/dummy_data/ShareFlex.csv</t>
+  </si>
+  <si>
+    <t>ZZ3</t>
   </si>
 </sst>
 </file>
@@ -1438,8 +1438,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1457,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1481,7 +1481,7 @@
     <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
@@ -1502,10 +1502,10 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="37"/>
@@ -1600,19 +1600,19 @@
     </row>
     <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="29"/>
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="30"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="28"/>
     </row>
@@ -1632,7 +1632,7 @@
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="36"/>
       <c r="C33" s="37"/>
@@ -1644,22 +1644,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>4</v>
@@ -1668,12 +1668,12 @@
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>4</v>
@@ -1682,30 +1682,30 @@
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="C37" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1727,7 @@
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B56" s="36"/>
       <c r="C56" s="37"/>
@@ -1739,52 +1739,52 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C57" s="17">
         <v>42005</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C58" s="17">
         <v>42011</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>47</v>
       </c>
       <c r="C59" s="4">
         <v>4</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="4">
         <v>1</v>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>208</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>209</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1826,7 +1826,7 @@
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B75" s="36"/>
       <c r="C75" s="37"/>
@@ -1841,35 +1841,35 @@
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>4</v>
@@ -1878,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,7 +1952,7 @@
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B98" s="36"/>
       <c r="C98" s="37"/>
@@ -1964,35 +1964,35 @@
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B101" s="30" t="s">
         <v>4</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E102" s="28" t="s">
         <v>0</v>
@@ -2012,12 +2012,12 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E103" s="28" t="s">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B124" s="36"/>
       <c r="C124" s="37"/>
@@ -2069,28 +2069,28 @@
         <v>2</v>
       </c>
       <c r="B125" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H125" s="11"/>
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B126" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E126" s="28" t="s">
         <v>0</v>
@@ -2105,16 +2105,16 @@
         <v>1</v>
       </c>
       <c r="B127" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H127" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,42 +2122,42 @@
         <v>3</v>
       </c>
       <c r="B128" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B129" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B130" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E130" s="28" t="s">
         <v>0</v>
@@ -2166,148 +2166,148 @@
         <v>0.05</v>
       </c>
       <c r="H130" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B131" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H131" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B132" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H132" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B133" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B134" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B136" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B136" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C136" s="19" t="s">
-        <v>200</v>
-      </c>
       <c r="D136" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H136" s="11"/>
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B137" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="B137" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C137" s="19" t="s">
-        <v>224</v>
-      </c>
       <c r="D137" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B138" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B139" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B140" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2392,27 +2392,27 @@
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B161" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C161" s="19" t="s">
         <v>219</v>
-      </c>
-      <c r="B161" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C161" s="19" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B162" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C162" s="19"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="28" t="s">
@@ -2422,12 +2422,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E164" s="28" t="s">
         <v>0</v>
@@ -2436,7 +2436,7 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,7 @@
     </row>
     <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="37"/>
@@ -2457,14 +2457,14 @@
     </row>
     <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B167" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C167" s="19"/>
       <c r="D167" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E167" s="28" t="s">
         <v>0</v>
@@ -2475,14 +2475,14 @@
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B168" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C168" s="19"/>
       <c r="D168" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E168" s="28" t="s">
         <v>0</v>
@@ -2493,14 +2493,14 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B169" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C169" s="19"/>
       <c r="D169" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E169" s="28" t="s">
         <v>0</v>
@@ -2509,19 +2509,19 @@
         <v>400</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B170" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C170" s="19"/>
       <c r="D170" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E170" s="28" t="s">
         <v>0</v>
@@ -2530,19 +2530,19 @@
         <v>0</v>
       </c>
       <c r="H170" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B171" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C171" s="19"/>
       <c r="D171" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E171" s="28" t="s">
         <v>0</v>
@@ -2589,10 +2589,10 @@
     </row>
     <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B181" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C181" s="19"/>
       <c r="D181" s="18"/>
@@ -2605,16 +2605,16 @@
     </row>
     <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B182" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E182" s="28" t="s">
         <v>0</v>
@@ -2625,16 +2625,16 @@
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B183" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E183" s="28" t="s">
         <v>0</v>
@@ -2643,21 +2643,21 @@
         <v>20</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B184" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>0</v>
@@ -2668,16 +2668,16 @@
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B185" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>0</v>
@@ -2688,14 +2688,14 @@
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B186" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C186" s="19"/>
       <c r="D186" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E186" s="28" t="s">
         <v>0</v>
@@ -2706,16 +2706,16 @@
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B187" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E187" s="28" t="s">
         <v>0</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C205" s="1"/>
       <c r="E205" s="28" t="s">
@@ -2795,12 +2795,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C206" s="1"/>
       <c r="E206" s="28" t="s">
@@ -2810,12 +2810,12 @@
         <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="28" t="s">
@@ -2825,7 +2825,7 @@
         <v>400</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2894,34 +2894,34 @@
     </row>
     <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B225" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C225" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D225" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E225" s="43" t="s">
         <v>4</v>
       </c>
       <c r="F225" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G225" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H225" s="40"/>
     </row>
     <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>0</v>
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>1</v>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2953,19 +2953,19 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>18</v>
+        <v>233</v>
       </c>
       <c r="F227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C228" s="4" t="b">
         <v>0</v>
@@ -2974,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F228" s="4" t="b">
         <v>0</v>
@@ -2986,7 +2986,7 @@
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -3007,7 +3007,7 @@
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -3016,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F231" s="4" t="b">
         <v>0</v>
@@ -3049,16 +3049,16 @@
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
@@ -3070,7 +3070,7 @@
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C233" s="4" t="b">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F233" s="4" t="b">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F235" s="4" t="b">
         <v>0</v>
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F236" s="4" t="b">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F237" s="4" t="b">
         <v>0</v>
@@ -3184,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F238" s="4" t="b">
         <v>0</v>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3238,16 +3238,16 @@
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E241" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C241" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D241" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E241" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F241" s="4" t="b">
         <v>0</v>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F242" s="4" t="b">
         <v>0</v>
@@ -3287,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F243" s="4" t="b">
         <v>0</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C244" s="4" t="b">
         <v>0</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F245" s="4" t="b">
         <v>0</v>
@@ -3342,7 +3342,7 @@
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3351,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="E246" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F246" s="4" t="b">
         <v>0</v>
@@ -3360,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3486,7 +3486,7 @@
     <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B274" s="36"/>
       <c r="C274" s="37"/>
@@ -3501,46 +3501,46 @@
         <v>2</v>
       </c>
       <c r="B275" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B276" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C276" s="5">
         <v>1</v>
       </c>
       <c r="H276" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B277" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B277" s="28" t="s">
-        <v>76</v>
-      </c>
       <c r="C277" s="5">
         <v>1</v>
       </c>
       <c r="H277" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B278" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C278" s="5">
         <v>1</v>
@@ -3576,7 +3576,7 @@
     <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B304" s="40"/>
       <c r="C304" s="42"/>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C305" s="31" t="s">
         <v>4</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C306" s="21" t="b">
         <v>1</v>
@@ -3604,7 +3604,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C307" s="21" t="b">
         <v>1</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C308" s="21" t="b">
         <v>1</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C309" s="21" t="b">
         <v>0</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C310" s="21" t="b">
         <v>1</v>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C311" s="21" t="b">
         <v>1</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C312" s="21" t="b">
         <v>0</v>
@@ -3652,7 +3652,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C313" s="21" t="b">
         <v>0</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C314" s="21" t="b">
         <v>0</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C315" s="21" t="b">
         <v>0</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C316" s="21" t="b">
         <v>1</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C317" s="21" t="b">
         <v>1</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C318" s="21" t="b">
         <v>1</v>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C319" s="21" t="b">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C320" s="21" t="b">
         <v>0</v>
@@ -3716,7 +3716,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3731,19 +3731,19 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C306:C320 C35:C36">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C226:D247 C79 C306:C320 C35:C36 F226:G247">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3805,7 +3805,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C306:C320 F226:G247 C226:D247</xm:sqref>
+          <xm:sqref>C306:C320 C226:D247 F226:G247</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
@@ -3884,19 +3884,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3904,19 +3904,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3924,40 +3924,40 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3982,51 +3982,51 @@
   <sheetData>
     <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="20" t="b">
         <v>1</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="20" t="b">
         <v>1</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="20" t="b">
         <v>0</v>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="20" t="b">
         <v>0</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="20" t="b">
         <v>1</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="20" t="b">
         <v>1</v>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="20" t="b">
         <v>0</v>
@@ -4355,7 +4355,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="20" t="b">
         <v>0</v>
@@ -4402,7 +4402,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="20" t="b">
         <v>0</v>
@@ -4449,7 +4449,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="20" t="b">
         <v>0</v>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="20" t="b">
         <v>1</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="20" t="b">
         <v>1</v>
@@ -4590,7 +4590,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="20" t="b">
         <v>1</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="20" t="b">
         <v>0</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="20" t="b">
         <v>0</v>
@@ -4734,10 +4734,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Heat demand can be covered by multiple units
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA9A141-710F-4B4C-B2E5-3E3ECCA9EF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61F03DD-8488-41C7-AE9D-0AF757DC6344}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="233">
   <si>
     <t>Default value</t>
   </si>
@@ -291,9 +294,6 @@
   </si>
   <si>
     <t>Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Hour 0 of the day is defined as midnight in timezone UTC+1</t>
@@ -1438,8 +1438,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1457,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1505,7 +1505,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="37"/>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="30"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="28"/>
     </row>
@@ -1632,7 +1632,7 @@
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="36"/>
       <c r="C33" s="37"/>
@@ -1650,7 +1650,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1692,20 +1692,18 @@
       <c r="B37" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1725,7 @@
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B56" s="36"/>
       <c r="C56" s="37"/>
@@ -1776,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,10 +1790,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1803,10 +1801,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>207</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>208</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1826,7 +1824,7 @@
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B75" s="36"/>
       <c r="C75" s="37"/>
@@ -1847,7 +1845,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>63</v>
@@ -1869,7 +1867,7 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>4</v>
@@ -1885,74 +1883,26 @@
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="C96" s="1"/>
-    </row>
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B98" s="36"/>
       <c r="C98" s="37"/>
@@ -1964,35 +1914,35 @@
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B101" s="30" t="s">
         <v>4</v>
@@ -2003,7 +1953,7 @@
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E102" s="28" t="s">
         <v>0</v>
@@ -2012,12 +1962,12 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E103" s="28" t="s">
         <v>0</v>
@@ -2026,7 +1976,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2004,7 @@
     </row>
     <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B124" s="36"/>
       <c r="C124" s="37"/>
@@ -2072,25 +2022,25 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H125" s="11"/>
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B126" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E126" s="28" t="s">
         <v>0</v>
@@ -2108,10 +2058,10 @@
         <v>35</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H127" s="11" t="s">
         <v>52</v>
@@ -2125,13 +2075,13 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2142,10 +2092,10 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2157,7 +2107,7 @@
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E130" s="28" t="s">
         <v>0</v>
@@ -2177,10 +2127,10 @@
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H131" s="11" t="s">
         <v>53</v>
@@ -2188,16 +2138,16 @@
     </row>
     <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B132" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H132" s="11" t="s">
         <v>54</v>
@@ -2205,16 +2155,16 @@
     </row>
     <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B133" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>55</v>
@@ -2222,92 +2172,92 @@
     </row>
     <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B134" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B135" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B136" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H136" s="11"/>
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B138" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B139" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B140" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2392,18 +2342,18 @@
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B161" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B162" s="29" t="s">
         <v>35</v>
@@ -2412,7 +2362,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="28" t="s">
@@ -2422,12 +2372,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E164" s="28" t="s">
         <v>0</v>
@@ -2436,7 +2386,7 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2445,7 +2395,7 @@
     </row>
     <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="37"/>
@@ -2457,14 +2407,14 @@
     </row>
     <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B167" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C167" s="19"/>
       <c r="D167" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E167" s="28" t="s">
         <v>0</v>
@@ -2475,14 +2425,14 @@
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B168" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C168" s="19"/>
       <c r="D168" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E168" s="28" t="s">
         <v>0</v>
@@ -2493,14 +2443,14 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B169" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C169" s="19"/>
       <c r="D169" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E169" s="28" t="s">
         <v>0</v>
@@ -2509,19 +2459,19 @@
         <v>400</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C170" s="19"/>
       <c r="D170" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E170" s="28" t="s">
         <v>0</v>
@@ -2530,19 +2480,19 @@
         <v>0</v>
       </c>
       <c r="H170" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C171" s="19"/>
       <c r="D171" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E171" s="28" t="s">
         <v>0</v>
@@ -2589,7 +2539,7 @@
     </row>
     <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B181" s="29" t="s">
         <v>35</v>
@@ -2605,16 +2555,16 @@
     </row>
     <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B182" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E182" s="28" t="s">
         <v>0</v>
@@ -2631,10 +2581,10 @@
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E183" s="28" t="s">
         <v>0</v>
@@ -2643,7 +2593,7 @@
         <v>20</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,10 +2604,10 @@
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>0</v>
@@ -2668,16 +2618,16 @@
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B185" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>0</v>
@@ -2688,14 +2638,14 @@
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B186" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C186" s="19"/>
       <c r="D186" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E186" s="28" t="s">
         <v>0</v>
@@ -2706,16 +2656,16 @@
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B187" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E187" s="28" t="s">
         <v>0</v>
@@ -2785,7 +2735,7 @@
     </row>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C205" s="1"/>
       <c r="E205" s="28" t="s">
@@ -2795,12 +2745,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C206" s="1"/>
       <c r="E206" s="28" t="s">
@@ -2810,12 +2760,12 @@
         <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="28" t="s">
@@ -2825,7 +2775,7 @@
         <v>400</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2894,25 +2844,25 @@
     </row>
     <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B225" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C225" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D225" s="44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E225" s="43" t="s">
         <v>4</v>
       </c>
       <c r="F225" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G225" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H225" s="40"/>
     </row>
@@ -2921,7 +2871,7 @@
         <v>50</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>0</v>
@@ -2930,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>1</v>
@@ -2944,7 +2894,7 @@
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2953,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>1</v>
@@ -2986,7 +2936,7 @@
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -3007,7 +2957,7 @@
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -3016,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -3037,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F231" s="4" t="b">
         <v>0</v>
@@ -3049,16 +2999,16 @@
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
@@ -3100,7 +3050,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3205,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3226,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3307,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3318,7 +3268,7 @@
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3330,7 +3280,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F245" s="4" t="b">
         <v>0</v>
@@ -3342,7 +3292,7 @@
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3360,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3374,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3576,7 +3526,7 @@
     <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B304" s="40"/>
       <c r="C304" s="42"/>
@@ -3588,7 +3538,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C305" s="31" t="s">
         <v>4</v>
@@ -3596,7 +3546,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C306" s="21" t="b">
         <v>1</v>
@@ -3604,7 +3554,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C307" s="21" t="b">
         <v>1</v>
@@ -3612,7 +3562,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C308" s="21" t="b">
         <v>1</v>
@@ -3620,7 +3570,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C309" s="21" t="b">
         <v>0</v>
@@ -3628,7 +3578,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C310" s="21" t="b">
         <v>1</v>
@@ -3636,7 +3586,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C311" s="21" t="b">
         <v>1</v>
@@ -3644,7 +3594,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C312" s="21" t="b">
         <v>0</v>
@@ -3652,7 +3602,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C313" s="21" t="b">
         <v>0</v>
@@ -3660,7 +3610,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C314" s="21" t="b">
         <v>0</v>
@@ -3668,7 +3618,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C315" s="21" t="b">
         <v>0</v>
@@ -3676,7 +3626,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C316" s="21" t="b">
         <v>1</v>
@@ -3684,7 +3634,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C317" s="21" t="b">
         <v>1</v>
@@ -3692,7 +3642,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C318" s="21" t="b">
         <v>1</v>
@@ -3700,7 +3650,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C319" s="21" t="b">
         <v>0</v>
@@ -3708,7 +3658,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C320" s="21" t="b">
         <v>0</v>
@@ -3716,7 +3666,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3732,18 +3682,18 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C226:D247 C79 C306:C320 C35:C36 F226:G247">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3893,10 +3843,10 @@
         <v>79</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3904,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -3913,10 +3863,10 @@
         <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3930,10 +3880,10 @@
         <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3944,12 +3894,12 @@
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>
@@ -3957,7 +3907,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3982,51 +3932,51 @@
   <sheetData>
     <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="20" t="b">
         <v>1</v>
@@ -4073,7 +4023,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="20" t="b">
         <v>1</v>
@@ -4120,7 +4070,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="20" t="b">
         <v>0</v>
@@ -4167,7 +4117,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="20" t="b">
         <v>0</v>
@@ -4214,7 +4164,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="20" t="b">
         <v>1</v>
@@ -4261,7 +4211,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="20" t="b">
         <v>1</v>
@@ -4308,7 +4258,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="20" t="b">
         <v>0</v>
@@ -4355,7 +4305,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="20" t="b">
         <v>0</v>
@@ -4402,7 +4352,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="20" t="b">
         <v>0</v>
@@ -4449,7 +4399,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="20" t="b">
         <v>0</v>
@@ -4496,7 +4446,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="20" t="b">
         <v>1</v>
@@ -4543,7 +4493,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="20" t="b">
         <v>1</v>
@@ -4590,7 +4540,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="20" t="b">
         <v>1</v>
@@ -4637,7 +4587,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="20" t="b">
         <v>0</v>
@@ -4684,7 +4634,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="20" t="b">
         <v>0</v>
@@ -4734,10 +4684,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
p2ht units properly assigned + Heating plots update
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61F03DD-8488-41C7-AE9D-0AF757DC6344}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580E427A-4867-4AFE-B020-4E98CAE63241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1438,8 +1438,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -3465,7 +3465,7 @@
         <v>75</v>
       </c>
       <c r="C276" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>77</v>
@@ -3479,7 +3479,7 @@
         <v>75</v>
       </c>
       <c r="C277" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Curtailment of renewable heat technologies now visible in plots
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580E427A-4867-4AFE-B020-4E98CAE63241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C039675D-AD1A-42EA-A2C5-E697C5635BF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1438,8 +1438,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,7 +3479,7 @@
         <v>75</v>
       </c>
       <c r="C277" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Fix for previous merge commit (ConfigTest.xlsx properly loading reserves)
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C039675D-AD1A-42EA-A2C5-E697C5635BF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E1485-E5C4-4053-A699-9875B1F8D934}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$78:$C$99</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="255">
   <si>
     <t>Default value</t>
   </si>
@@ -395,9 +395,6 @@
     <t>OTH</t>
   </si>
   <si>
-    <t>Participation to reserve markets</t>
-  </si>
-  <si>
     <t>Price of Nuclear</t>
   </si>
   <si>
@@ -735,6 +732,75 @@
   </si>
   <si>
     <t>ZZ3</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Probabilistic</t>
+  </si>
+  <si>
+    <t>Exogenous</t>
+  </si>
+  <si>
+    <t>Participation to reserve markets (CHP units)</t>
+  </si>
+  <si>
+    <t>Participation to reserve markets (Non-CHP units)</t>
+  </si>
+  <si>
+    <t>P2HT</t>
+  </si>
+  <si>
+    <t>ABHP</t>
+  </si>
+  <si>
+    <t>ASHP</t>
+  </si>
+  <si>
+    <t>GSHP</t>
+  </si>
+  <si>
+    <t>HYHP</t>
+  </si>
+  <si>
+    <t>WSHP</t>
+  </si>
+  <si>
+    <t>REHE</t>
+  </si>
+  <si>
+    <t>ALKE</t>
+  </si>
+  <si>
+    <t>PEME</t>
+  </si>
+  <si>
+    <t>SOXE</t>
+  </si>
+  <si>
+    <t>PEFC</t>
+  </si>
+  <si>
+    <t>DMFC</t>
+  </si>
+  <si>
+    <t>ALFC</t>
+  </si>
+  <si>
+    <t>PAFC</t>
+  </si>
+  <si>
+    <t>MCFC</t>
+  </si>
+  <si>
+    <t>SCSP</t>
+  </si>
+  <si>
+    <t>SOFC</t>
+  </si>
+  <si>
+    <t>REFC</t>
   </si>
 </sst>
 </file>
@@ -895,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1018,9 +1084,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1049,7 +1112,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1438,8 +1557,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="C278" sqref="C278"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,16 +1575,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1480,15 +1599,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1504,78 +1623,78 @@
       <c r="A6" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="B6" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
     </row>
     <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -1588,7 +1707,7 @@
     </row>
     <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="37"/>
@@ -1606,13 +1725,13 @@
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" s="30"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18" s="28"/>
     </row>
@@ -1632,7 +1751,7 @@
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B33" s="36"/>
       <c r="C33" s="37"/>
@@ -1650,7 +1769,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1696,7 +1815,7 @@
     </row>
     <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>85</v>
@@ -1725,7 +1844,7 @@
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" s="36"/>
       <c r="C56" s="37"/>
@@ -1790,10 +1909,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1801,10 +1920,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>206</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>207</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1824,7 +1943,7 @@
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" s="36"/>
       <c r="C75" s="37"/>
@@ -1845,7 +1964,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>63</v>
@@ -1859,7 +1978,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>58</v>
+        <v>233</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -1867,7 +1986,7 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>4</v>
@@ -1902,7 +2021,7 @@
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B98" s="36"/>
       <c r="C98" s="37"/>
@@ -1914,35 +2033,35 @@
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B101" s="30" t="s">
         <v>4</v>
@@ -1953,7 +2072,7 @@
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E102" s="28" t="s">
         <v>0</v>
@@ -1962,12 +2081,12 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E103" s="28" t="s">
         <v>0</v>
@@ -1976,7 +2095,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2123,7 @@
     </row>
     <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B124" s="36"/>
       <c r="C124" s="37"/>
@@ -2022,7 +2141,7 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>87</v>
@@ -2031,13 +2150,13 @@
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B126" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D126" s="18" t="s">
         <v>87</v>
@@ -2058,7 +2177,7 @@
         <v>35</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D127" s="18" t="s">
         <v>87</v>
@@ -2075,13 +2194,13 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,7 +2211,7 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>87</v>
@@ -2127,7 +2246,7 @@
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>87</v>
@@ -2144,7 +2263,7 @@
         <v>35</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D132" s="18" t="s">
         <v>87</v>
@@ -2155,13 +2274,13 @@
     </row>
     <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B133" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>87</v>
@@ -2172,13 +2291,13 @@
     </row>
     <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B134" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D134" s="18" t="s">
         <v>87</v>
@@ -2186,13 +2305,13 @@
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B135" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>87</v>
@@ -2200,13 +2319,13 @@
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B136" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>87</v>
@@ -2215,13 +2334,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>87</v>
@@ -2229,35 +2348,35 @@
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B138" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B139" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B140" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,18 +2461,18 @@
     </row>
     <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B161" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B162" s="29" t="s">
         <v>35</v>
@@ -2362,7 +2481,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="28" t="s">
@@ -2372,12 +2491,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E164" s="28" t="s">
         <v>0</v>
@@ -2386,7 +2505,7 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2395,7 +2514,7 @@
     </row>
     <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="37"/>
@@ -2407,7 +2526,7 @@
     </row>
     <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B167" s="29" t="s">
         <v>35</v>
@@ -2425,7 +2544,7 @@
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B168" s="29" t="s">
         <v>35</v>
@@ -2443,7 +2562,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B169" s="29" t="s">
         <v>35</v>
@@ -2459,12 +2578,12 @@
         <v>400</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>35</v>
@@ -2480,12 +2599,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>35</v>
@@ -2539,7 +2658,7 @@
     </row>
     <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B181" s="29" t="s">
         <v>35</v>
@@ -2561,7 +2680,7 @@
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D182" s="18" t="s">
         <v>87</v>
@@ -2581,7 +2700,7 @@
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D183" s="18" t="s">
         <v>87</v>
@@ -2593,7 +2712,7 @@
         <v>20</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2604,7 +2723,7 @@
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D184" s="18" t="s">
         <v>87</v>
@@ -2618,13 +2737,13 @@
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B185" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D185" s="18" t="s">
         <v>87</v>
@@ -2638,7 +2757,7 @@
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B186" s="29" t="s">
         <v>35</v>
@@ -2656,13 +2775,13 @@
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B187" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D187" s="18" t="s">
         <v>87</v>
@@ -2735,7 +2854,7 @@
     </row>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C205" s="1"/>
       <c r="E205" s="28" t="s">
@@ -2745,12 +2864,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C206" s="1"/>
       <c r="E206" s="28" t="s">
@@ -2760,12 +2879,12 @@
         <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="28" t="s">
@@ -2775,7 +2894,7 @@
         <v>400</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2844,25 +2963,25 @@
     </row>
     <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="B225" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B225" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C225" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="D225" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="E225" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="D225" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E225" s="42" t="s">
         <v>4</v>
       </c>
       <c r="F225" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G225" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H225" s="40"/>
     </row>
@@ -2871,7 +2990,7 @@
         <v>50</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>0</v>
@@ -2880,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>1</v>
@@ -2890,11 +3009,11 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="47" t="s">
+      <c r="A227" s="46" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2903,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>1</v>
@@ -2913,7 +3032,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="47"/>
+      <c r="A228" s="46"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -2934,9 +3053,9 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="47"/>
+      <c r="A229" s="46"/>
       <c r="B229" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -2955,9 +3074,9 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="47"/>
+      <c r="A230" s="46"/>
       <c r="B230" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -2966,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -2976,7 +3095,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="47"/>
+      <c r="A231" s="46"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -2987,29 +3106,29 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F231" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G231" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="46"/>
+      <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F231" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G231" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="47"/>
-      <c r="B232" s="6" t="s">
+      <c r="C232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
       </c>
@@ -3018,7 +3137,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="47"/>
+      <c r="A233" s="46"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3039,7 +3158,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="47"/>
+      <c r="A234" s="46"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3050,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3060,7 +3179,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="47"/>
+      <c r="A235" s="46"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3081,7 +3200,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="47"/>
+      <c r="A236" s="46"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3102,7 +3221,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="47"/>
+      <c r="A237" s="46"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3123,7 +3242,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="47"/>
+      <c r="A238" s="46"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3144,7 +3263,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="47"/>
+      <c r="A239" s="46"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3155,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3165,7 +3284,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="47"/>
+      <c r="A240" s="46"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3176,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3186,7 +3305,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="47"/>
+      <c r="A241" s="46"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3257,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3267,8 +3386,8 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="50" t="s">
-        <v>171</v>
+      <c r="A245" s="49" t="s">
+        <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3280,19 +3399,19 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F245" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G245" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="49"/>
+      <c r="B246" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="F245" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G245" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="50"/>
-      <c r="B246" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3310,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3324,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3496,177 +3615,337 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="9"/>
-      <c r="C302" s="14"/>
-    </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A298" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B298" s="36"/>
+      <c r="C298" s="37"/>
+      <c r="D298" s="36"/>
+      <c r="E298" s="36"/>
+      <c r="F298" s="36"/>
+      <c r="G298" s="36"/>
+      <c r="H298" s="36"/>
+    </row>
+    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C299" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D299" s="41"/>
+      <c r="E299" s="41"/>
+      <c r="F299" s="41"/>
+      <c r="G299" s="41"/>
+      <c r="H299" s="41"/>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B300" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C300" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B301" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C301" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2"/>
+      <c r="B302" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C302" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D302" s="1"/>
+      <c r="E302" s="1"/>
+      <c r="F302" s="1"/>
+      <c r="G302" s="1"/>
+      <c r="H302" s="1"/>
+    </row>
+    <row r="303" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="2"/>
+      <c r="B303" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C303" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D303" s="1"/>
+      <c r="E303" s="1"/>
+      <c r="F303" s="1"/>
+      <c r="G303" s="1"/>
+      <c r="H303" s="1"/>
+    </row>
     <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="B304" s="40"/>
-      <c r="C304" s="42"/>
-      <c r="D304" s="40"/>
-      <c r="E304" s="40"/>
-      <c r="F304" s="40"/>
-      <c r="G304" s="40"/>
-      <c r="H304" s="40"/>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="2"/>
+      <c r="B304" s="1"/>
+      <c r="C304" s="13"/>
+      <c r="D304" s="1"/>
+      <c r="E304" s="1"/>
+      <c r="F304" s="1"/>
+      <c r="G304" s="1"/>
+      <c r="H304" s="1"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>119</v>
+        <v>236</v>
       </c>
       <c r="C305" s="31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F305" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
         <v>90</v>
       </c>
       <c r="C306" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E306" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="F306" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
         <v>91</v>
       </c>
       <c r="C307" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E307" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="F307" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
         <v>92</v>
       </c>
       <c r="C308" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E308" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="F308" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
         <v>93</v>
       </c>
       <c r="C309" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E309" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F309" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
         <v>94</v>
       </c>
       <c r="C310" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E310" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="F310" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C311" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E311" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F311" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
         <v>96</v>
       </c>
       <c r="C312" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E312" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="F312" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C313" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E313" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="F313" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
         <v>98</v>
       </c>
       <c r="C314" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E314" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F314" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
         <v>99</v>
       </c>
       <c r="C315" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E315" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="F315" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
         <v>100</v>
       </c>
       <c r="C316" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E316" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="F316" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C317" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E317" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F317" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C318" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E318" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F318" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
         <v>103</v>
       </c>
       <c r="C319" s="21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E319" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="F319" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C320" s="21" t="b">
         <v>0</v>
       </c>
+      <c r="E320" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="F320" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B321" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="F321" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E322" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F322" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3681,20 +3960,52 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 C79 C306:C320 C35:C36 F226:G247">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C226:D247 C79 C35:C36 F226:G247">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F322 C306:C321">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C300:C303">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F306:F312">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F313:F321">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="547" yWindow="733" count="35">
@@ -3755,7 +4066,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C306:C320 C226:D247 F226:G247</xm:sqref>
+          <xm:sqref>F226:G247 C226:D247</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
@@ -3817,7 +4128,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3843,10 +4154,10 @@
         <v>79</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3854,7 +4165,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -3863,10 +4174,10 @@
         <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3876,30 +4187,39 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
       <c r="D3" t="s">
         <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>44</v>
       </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
       <c r="D4" t="s">
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>234</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>
@@ -3907,7 +4227,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4684,10 +5004,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Curtailment costs included in the objective function
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E1485-E5C4-4053-A699-9875B1F8D934}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A5469-7819-4C34-A6C8-0966A8FEEEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="256">
   <si>
     <t>Default value</t>
   </si>
@@ -801,6 +801,9 @@
   </si>
   <si>
     <t>REFC</t>
+  </si>
+  <si>
+    <t>Curtailment Cost</t>
   </si>
 </sst>
 </file>
@@ -1557,8 +1560,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,9 +2623,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="25"/>
-      <c r="C172" s="27"/>
+    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B172" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E172" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F172" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
@@ -3977,34 +3994,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F322 C306:C321">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C300:C303">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F313:F321">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4019,14 +4036,14 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C37" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F171" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F172" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
@@ -5004,10 +5021,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ammonia added as fuel type, updates to figures
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A5469-7819-4C34-A6C8-0966A8FEEEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD624C73-DA90-4701-AEAC-48287865EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="257">
   <si>
     <t>Default value</t>
   </si>
@@ -804,6 +804,9 @@
   </si>
   <si>
     <t>Curtailment Cost</t>
+  </si>
+  <si>
+    <t>Price of Ammonia</t>
   </si>
 </sst>
 </file>
@@ -1560,8 +1563,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A183" sqref="A183"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="5">
-        <v>7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2560,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -2620,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="5">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2686,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="F181" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2706,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="F182" s="5">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2726,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="F183" s="5">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H183" s="1" t="s">
         <v>122</v>
@@ -2749,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="F184" s="5">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2769,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="F185" s="5">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2787,7 +2790,7 @@
         <v>0</v>
       </c>
       <c r="F186" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2807,14 +2810,27 @@
         <v>0</v>
       </c>
       <c r="F187" s="5">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="25"/>
-      <c r="C188" s="27"/>
-    </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="A188" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="B188" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C188" s="19"/>
+      <c r="D188" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E188" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>76</v>
+      </c>
+    </row>
     <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4036,7 +4052,7 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F188 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>

</xml_diff>

<commit_message>
feat: added h2 zones
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD624C73-DA90-4701-AEAC-48287865EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC402EDA-8715-4F7E-B73E-35A27E737E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="F180" sqref="F180"/>
+      <selection activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>100</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(gams): Storage balance equation $(ord(i) > 1) properly defined
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC402EDA-8715-4F7E-B73E-35A27E737E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA08C0-245E-41E0-8C07-60798049A85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1563,8 +1563,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="F172" sqref="F172"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1</v>
+        <v>401</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -3606,7 +3606,7 @@
         <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -3617,7 +3617,7 @@
         <v>75</v>
       </c>
       <c r="C276" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
fix(bugs): minor bug fixes for outdated pandas functions
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA08C0-245E-41E0-8C07-60798049A85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76F6198-935E-4A1F-BC13-56ACF0E20004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="C276" sqref="C276"/>
+      <selection activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,7 +3606,7 @@
         <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -3617,7 +3617,7 @@
         <v>75</v>
       </c>
       <c r="C276" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>77</v>
@@ -3631,7 +3631,7 @@
         <v>75</v>
       </c>
       <c r="C277" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
fix(build): initial power now assigned based on the residual load + minor cleanup
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76F6198-935E-4A1F-BC13-56ACF0E20004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB8CBA-83FC-484F-9CFA-8B70BD21329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="256">
   <si>
     <t>Default value</t>
   </si>
@@ -687,9 +687,6 @@
   </si>
   <si>
     <t>Reserves Up</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/Reserve2U.csv</t>
   </si>
   <si>
     <t>Price of Unserved H2</t>
@@ -967,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1039,15 +1036,6 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1090,14 +1078,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1563,8 +1545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="C277" sqref="C277"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,16 +1563,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="A1" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1603,17 +1585,17 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="48" t="s">
+    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1626,81 +1608,81 @@
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -1711,35 +1693,35 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="26"/>
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="25"/>
     </row>
     <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1755,23 +1737,23 @@
     <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1786,7 +1768,7 @@
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="4" t="b">
@@ -1800,7 +1782,7 @@
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="4" t="b">
@@ -1814,7 +1796,7 @@
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="26" t="s">
         <v>85</v>
       </c>
       <c r="C37" s="4"/>
@@ -1823,7 +1805,7 @@
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="26" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="4"/>
@@ -1848,23 +1830,23 @@
     <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C57" s="17">
@@ -1878,7 +1860,7 @@
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C58" s="17">
@@ -1892,7 +1874,7 @@
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="4">
@@ -1906,7 +1888,7 @@
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C60" s="4">
@@ -1917,7 +1899,7 @@
       <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="25" t="s">
         <v>206</v>
       </c>
       <c r="C61" s="4">
@@ -1928,7 +1910,7 @@
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="25" t="s">
         <v>206</v>
       </c>
       <c r="C62" s="4">
@@ -1947,17 +1929,17 @@
     <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
+    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33"/>
     </row>
     <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
@@ -1966,7 +1948,7 @@
       <c r="A77" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -1980,11 +1962,11 @@
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="30" t="s">
+      <c r="B78" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>233</v>
+        <v>58</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -1994,7 +1976,7 @@
       <c r="A79" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="4" t="b">
@@ -2025,23 +2007,23 @@
     <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="35" t="s">
+    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B98" s="36"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="36"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="33"/>
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B99" s="30" t="s">
+      <c r="B99" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -2055,7 +2037,7 @@
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B100" s="30" t="s">
+      <c r="B100" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -2069,7 +2051,7 @@
       <c r="A101" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B101" s="30" t="s">
+      <c r="B101" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="4" t="b">
@@ -2077,10 +2059,10 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
+      <c r="A102" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="E102" s="28" t="s">
+      <c r="E102" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F102" s="5">
@@ -2091,10 +2073,10 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="E103" s="28" t="s">
+      <c r="E103" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F103" s="5">
@@ -2127,23 +2109,23 @@
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="35" t="s">
+    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="B124" s="36"/>
-      <c r="C124" s="37"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
-      <c r="F124" s="36"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="36"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="34"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33"/>
+      <c r="G124" s="33"/>
+      <c r="H124" s="33"/>
     </row>
     <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="29" t="s">
+      <c r="B125" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
@@ -2158,16 +2140,16 @@
       <c r="A126" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B126" s="29" t="s">
+      <c r="B126" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D126" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E126" s="28" t="s">
+      <c r="E126" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F126" s="5">
@@ -2179,11 +2161,11 @@
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B127" s="29" t="s">
+      <c r="B127" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D127" s="18" t="s">
         <v>87</v>
@@ -2196,11 +2178,11 @@
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="29" t="s">
+      <c r="B128" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
@@ -2213,7 +2195,7 @@
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B129" s="29" t="s">
+      <c r="B129" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
@@ -2227,14 +2209,14 @@
       <c r="A130" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B130" s="29" t="s">
+      <c r="B130" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E130" s="28" t="s">
+      <c r="E130" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F130" s="5">
@@ -2248,7 +2230,7 @@
       <c r="A131" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B131" s="29" t="s">
+      <c r="B131" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
@@ -2265,7 +2247,7 @@
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B132" s="29" t="s">
+      <c r="B132" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C132" s="19" t="s">
@@ -2282,7 +2264,7 @@
       <c r="A133" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B133" s="29" t="s">
+      <c r="B133" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C133" s="19" t="s">
@@ -2299,7 +2281,7 @@
       <c r="A134" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B134" s="29" t="s">
+      <c r="B134" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C134" s="19" t="s">
@@ -2313,7 +2295,7 @@
       <c r="A135" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B135" s="29" t="s">
+      <c r="B135" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
@@ -2327,7 +2309,7 @@
       <c r="A136" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B136" s="29" t="s">
+      <c r="B136" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
@@ -2340,147 +2322,85 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B137" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="B137" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C137" s="19" t="s">
-        <v>221</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="25" t="s">
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B138" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C138" s="19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B138" s="29" t="s">
+      <c r="B139" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C138" s="19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="25" t="s">
+      <c r="C139" s="19" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B139" s="29" t="s">
+      <c r="B140" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="19" t="s">
+      <c r="C140" s="19" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="B140" s="29" t="s">
+    <row r="141" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B161" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C140" s="19" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="25"/>
-      <c r="C141" s="27"/>
-    </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="25"/>
-      <c r="C142" s="27"/>
-    </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="25"/>
-      <c r="C143" s="27"/>
-    </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
-      <c r="C144" s="27"/>
-    </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
-      <c r="C145" s="27"/>
-    </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="25"/>
-      <c r="C146" s="27"/>
-    </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="25"/>
-      <c r="C147" s="27"/>
-    </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="25"/>
-      <c r="C148" s="27"/>
-    </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="25"/>
-      <c r="C149" s="27"/>
-    </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="25"/>
-      <c r="C150" s="27"/>
-    </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="25"/>
-      <c r="C151" s="27"/>
-    </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="25"/>
-      <c r="C152" s="27"/>
-    </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="25"/>
-      <c r="C153" s="27"/>
-    </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="25"/>
-      <c r="C154" s="27"/>
-    </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="25"/>
-      <c r="C155" s="27"/>
-    </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="25"/>
-      <c r="C156" s="27"/>
-    </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="25"/>
-      <c r="C157" s="27"/>
-    </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="25"/>
-      <c r="C158" s="27"/>
-    </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="25"/>
-      <c r="C159" s="27"/>
-    </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="25"/>
-      <c r="C160" s="27"/>
-    </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="B161" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C161" s="19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="25" t="s">
+      <c r="C161" s="19"/>
+    </row>
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B162" s="29" t="s">
+      <c r="B162" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C162" s="19"/>
@@ -2490,7 +2410,7 @@
         <v>209</v>
       </c>
       <c r="C163" s="1"/>
-      <c r="E163" s="28" t="s">
+      <c r="E163" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F163" s="5">
@@ -2504,7 +2424,7 @@
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E164" s="28" t="s">
+      <c r="E164" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F164" s="5">
@@ -2514,34 +2434,31 @@
         <v>208</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="25"/>
-      <c r="C165" s="27"/>
-    </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="35" t="s">
+    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B166" s="36"/>
-      <c r="C166" s="37"/>
-      <c r="D166" s="36"/>
-      <c r="E166" s="36"/>
-      <c r="F166" s="36"/>
-      <c r="G166" s="36"/>
-      <c r="H166" s="36"/>
+      <c r="B166" s="33"/>
+      <c r="C166" s="34"/>
+      <c r="D166" s="33"/>
+      <c r="E166" s="33"/>
+      <c r="F166" s="33"/>
+      <c r="G166" s="33"/>
+      <c r="H166" s="33"/>
     </row>
     <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B167" s="29" t="s">
+      <c r="B167" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C167" s="19"/>
       <c r="D167" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E167" s="28" t="s">
+      <c r="E167" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F167" s="5">
@@ -2552,14 +2469,14 @@
       <c r="A168" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B168" s="29" t="s">
+      <c r="B168" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C168" s="19"/>
       <c r="D168" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E168" s="28" t="s">
+      <c r="E168" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F168" s="5">
@@ -2570,14 +2487,14 @@
       <c r="A169" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B169" s="29" t="s">
+      <c r="B169" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C169" s="19"/>
       <c r="D169" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E169" s="28" t="s">
+      <c r="E169" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F169" s="5">
@@ -2587,105 +2504,81 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B170" s="29" t="s">
+      <c r="B170" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C170" s="19"/>
       <c r="D170" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E170" s="28" t="s">
+      <c r="E170" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F170" s="5">
         <v>0</v>
       </c>
-      <c r="H170" s="26" t="s">
+      <c r="H170" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B171" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B171" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C171" s="19"/>
       <c r="D171" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E171" s="28" t="s">
+      <c r="E171" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B172" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="B172" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C172" s="19"/>
       <c r="D172" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E172" s="28" t="s">
+      <c r="E172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F172" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="25"/>
-      <c r="C173" s="27"/>
-    </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="25"/>
-      <c r="C174" s="27"/>
-    </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="25"/>
-      <c r="C175" s="27"/>
-    </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="25"/>
-      <c r="C176" s="27"/>
-    </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="25"/>
-      <c r="C177" s="27"/>
-    </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="25"/>
-      <c r="C178" s="27"/>
-    </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="25"/>
-      <c r="C179" s="27"/>
-    </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="25"/>
-      <c r="C180" s="27"/>
-    </row>
+    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B181" s="29" t="s">
+      <c r="B181" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C181" s="19"/>
       <c r="D181" s="18"/>
-      <c r="E181" s="28" t="s">
+      <c r="E181" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F181" s="5">
@@ -2696,7 +2589,7 @@
       <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B182" s="29" t="s">
+      <c r="B182" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
@@ -2705,7 +2598,7 @@
       <c r="D182" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E182" s="28" t="s">
+      <c r="E182" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F182" s="5">
@@ -2716,7 +2609,7 @@
       <c r="A183" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B183" s="29" t="s">
+      <c r="B183" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
@@ -2725,7 +2618,7 @@
       <c r="D183" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E183" s="28" t="s">
+      <c r="E183" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F183" s="5">
@@ -2739,7 +2632,7 @@
       <c r="A184" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B184" s="29" t="s">
+      <c r="B184" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
@@ -2748,7 +2641,7 @@
       <c r="D184" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E184" s="28" t="s">
+      <c r="E184" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F184" s="5">
@@ -2759,7 +2652,7 @@
       <c r="A185" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B185" s="29" t="s">
+      <c r="B185" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
@@ -2768,7 +2661,7 @@
       <c r="D185" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E185" s="28" t="s">
+      <c r="E185" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F185" s="5">
@@ -2779,14 +2672,14 @@
       <c r="A186" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B186" s="29" t="s">
+      <c r="B186" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C186" s="19"/>
       <c r="D186" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E186" s="28" t="s">
+      <c r="E186" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F186" s="5">
@@ -2797,7 +2690,7 @@
       <c r="A187" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B187" s="29" t="s">
+      <c r="B187" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
@@ -2806,25 +2699,25 @@
       <c r="D187" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E187" s="28" t="s">
+      <c r="E187" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F187" s="5">
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="B188" s="29" t="s">
+    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B188" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C188" s="19"/>
       <c r="D188" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E188" s="28" t="s">
+      <c r="E188" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F188" s="5">
@@ -2833,64 +2726,25 @@
     </row>
     <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="25"/>
-      <c r="C192" s="27"/>
-    </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="25"/>
-      <c r="C193" s="27"/>
-    </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="25"/>
-      <c r="C194" s="27"/>
-    </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="25"/>
-      <c r="C195" s="27"/>
-    </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="25"/>
-      <c r="C196" s="27"/>
-    </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="25"/>
-      <c r="C197" s="27"/>
-    </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="25"/>
-      <c r="C198" s="27"/>
-    </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="25"/>
-      <c r="C199" s="27"/>
-    </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="25"/>
-      <c r="C200" s="27"/>
-    </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="25"/>
-      <c r="C201" s="27"/>
-    </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="25"/>
-      <c r="C202" s="27"/>
-    </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="25"/>
-      <c r="C203" s="27"/>
-    </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="25"/>
-      <c r="C204" s="27"/>
-    </row>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>144</v>
       </c>
       <c r="C205" s="1"/>
-      <c r="E205" s="28" t="s">
+      <c r="E205" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F205" s="24">
@@ -2905,7 +2759,7 @@
         <v>142</v>
       </c>
       <c r="C206" s="1"/>
-      <c r="E206" s="28" t="s">
+      <c r="E206" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F206" s="5">
@@ -2920,7 +2774,7 @@
         <v>145</v>
       </c>
       <c r="C207" s="1"/>
-      <c r="E207" s="28" t="s">
+      <c r="E207" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F207" s="5">
@@ -2930,93 +2784,48 @@
         <v>147</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="25"/>
-      <c r="C209" s="27"/>
-    </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="25"/>
-      <c r="C210" s="27"/>
-    </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="25"/>
-      <c r="C211" s="27"/>
-    </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="25"/>
-      <c r="C212" s="27"/>
-    </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="25"/>
-      <c r="C213" s="27"/>
-    </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="25"/>
-      <c r="C214" s="27"/>
-    </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="25"/>
-      <c r="C215" s="27"/>
-    </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="25"/>
-      <c r="C216" s="27"/>
-    </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="25"/>
-      <c r="C217" s="27"/>
-    </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="25"/>
-      <c r="C218" s="27"/>
-    </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="25"/>
-      <c r="C219" s="27"/>
-    </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="25"/>
-      <c r="C220" s="27"/>
-    </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="25"/>
-      <c r="C221" s="27"/>
-    </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="25"/>
-      <c r="C222" s="27"/>
-    </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="25"/>
-      <c r="C223" s="27"/>
-    </row>
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="39" t="s">
+    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="B225" s="42" t="s">
+      <c r="B225" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C225" s="39" t="s">
+      <c r="C225" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D225" s="43" t="s">
+      <c r="D225" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="E225" s="42" t="s">
+      <c r="E225" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F225" s="39" t="s">
+      <c r="F225" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="G225" s="39" t="s">
+      <c r="G225" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="H225" s="40"/>
+      <c r="H225" s="37"/>
     </row>
     <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
@@ -3042,7 +2851,7 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="46" t="s">
+      <c r="A227" s="41" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -3055,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>1</v>
@@ -3065,7 +2874,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="46"/>
+      <c r="A228" s="41"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -3086,7 +2895,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="46"/>
+      <c r="A229" s="41"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
       </c>
@@ -3107,7 +2916,7 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="46"/>
+      <c r="A230" s="41"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
       </c>
@@ -3128,7 +2937,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="46"/>
+      <c r="A231" s="41"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3149,7 +2958,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="46"/>
+      <c r="A232" s="41"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
@@ -3170,7 +2979,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="46"/>
+      <c r="A233" s="41"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3191,7 +3000,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="46"/>
+      <c r="A234" s="41"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3212,7 +3021,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="46"/>
+      <c r="A235" s="41"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3233,7 +3042,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="46"/>
+      <c r="A236" s="41"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3254,7 +3063,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="46"/>
+      <c r="A237" s="41"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3275,7 +3084,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="46"/>
+      <c r="A238" s="41"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3296,7 +3105,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="46"/>
+      <c r="A239" s="41"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3317,7 +3126,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="46"/>
+      <c r="A240" s="41"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3338,7 +3147,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="46"/>
+      <c r="A241" s="41"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3419,7 +3228,7 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="49" t="s">
+      <c r="A245" s="44" t="s">
         <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3442,7 +3251,7 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="49"/>
+      <c r="A246" s="44"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
       </c>
@@ -3485,139 +3294,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="25"/>
-      <c r="C248" s="27"/>
-    </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="25"/>
-      <c r="C249" s="27"/>
-    </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="25"/>
-      <c r="C250" s="27"/>
-    </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="25"/>
-      <c r="C251" s="27"/>
-    </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="25"/>
-      <c r="C252" s="27"/>
-    </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="25"/>
-      <c r="C253" s="27"/>
-    </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="25"/>
-      <c r="C254" s="27"/>
-    </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="25"/>
-      <c r="C255" s="27"/>
-    </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="25"/>
-      <c r="C256" s="27"/>
-    </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="25"/>
-      <c r="C257" s="27"/>
-    </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="25"/>
-      <c r="C258" s="27"/>
-    </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="25"/>
-      <c r="C259" s="27"/>
-    </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="25"/>
-      <c r="C260" s="27"/>
-    </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="25"/>
-      <c r="C261" s="27"/>
-    </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="25"/>
-      <c r="C262" s="27"/>
-    </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="25"/>
-      <c r="C263" s="27"/>
-    </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="25"/>
-      <c r="C264" s="27"/>
-    </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="25"/>
-      <c r="C265" s="27"/>
-    </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="25"/>
-      <c r="C266" s="27"/>
-    </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="25"/>
-      <c r="C267" s="27"/>
-    </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="25"/>
-      <c r="C268" s="27"/>
-    </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="25"/>
-      <c r="C269" s="27"/>
-    </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="25"/>
-      <c r="C270" s="27"/>
-    </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="25"/>
-      <c r="C271" s="27"/>
-    </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="25"/>
-      <c r="C272" s="27"/>
-    </row>
+    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="35" t="s">
+    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B274" s="36"/>
-      <c r="C274" s="37"/>
-      <c r="D274" s="36"/>
-      <c r="E274" s="36"/>
-      <c r="F274" s="36"/>
-      <c r="G274" s="36"/>
-      <c r="H274" s="36"/>
+      <c r="B274" s="33"/>
+      <c r="C274" s="34"/>
+      <c r="D274" s="33"/>
+      <c r="E274" s="33"/>
+      <c r="F274" s="33"/>
+      <c r="G274" s="33"/>
+      <c r="H274" s="33"/>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B275" s="28" t="s">
+      <c r="B275" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B276" s="28" t="s">
+      <c r="B276" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C276" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>77</v>
@@ -3627,11 +3361,11 @@
       <c r="A277" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B277" s="28" t="s">
+      <c r="B277" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C277" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>78</v>
@@ -3641,7 +3375,7 @@
       <c r="A278" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B278" s="28" t="s">
+      <c r="B278" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C278" s="5">
@@ -3655,29 +3389,29 @@
     <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A298" s="35" t="s">
+      <c r="A298" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B298" s="36"/>
-      <c r="C298" s="37"/>
-      <c r="D298" s="36"/>
-      <c r="E298" s="36"/>
-      <c r="F298" s="36"/>
-      <c r="G298" s="36"/>
-      <c r="H298" s="36"/>
+      <c r="B298" s="33"/>
+      <c r="C298" s="34"/>
+      <c r="D298" s="33"/>
+      <c r="E298" s="33"/>
+      <c r="F298" s="33"/>
+      <c r="G298" s="33"/>
+      <c r="H298" s="33"/>
     </row>
     <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C299" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C299" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="41"/>
-      <c r="E299" s="41"/>
-      <c r="F299" s="41"/>
-      <c r="G299" s="41"/>
-      <c r="H299" s="41"/>
+      <c r="D299" s="38"/>
+      <c r="E299" s="38"/>
+      <c r="F299" s="38"/>
+      <c r="G299" s="38"/>
+      <c r="H299" s="38"/>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
@@ -3695,35 +3429,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="2"/>
+    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C302" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="D302" s="1"/>
-      <c r="E302" s="1"/>
-      <c r="F302" s="1"/>
-      <c r="G302" s="1"/>
-      <c r="H302" s="1"/>
-    </row>
-    <row r="303" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A303" s="2"/>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B303" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C303" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="D303" s="1"/>
-      <c r="E303" s="1"/>
-      <c r="F303" s="1"/>
-      <c r="G303" s="1"/>
-      <c r="H303" s="1"/>
-    </row>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="C304" s="13"/>
@@ -3735,12 +3457,12 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C305" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C305" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F305" s="31" t="s">
+      <c r="F305" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3752,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F306" s="21" t="b">
         <v>1</v>
@@ -3766,7 +3488,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F307" s="21" t="b">
         <v>1</v>
@@ -3780,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F308" s="21" t="b">
         <v>1</v>
@@ -3794,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="E309" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F309" s="21" t="b">
         <v>1</v>
@@ -3808,7 +3530,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F310" s="21" t="b">
         <v>1</v>
@@ -3822,7 +3544,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F311" s="21" t="b">
         <v>1</v>
@@ -3836,7 +3558,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F312" s="21" t="b">
         <v>1</v>
@@ -3850,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F313" s="21" t="b">
         <v>0</v>
@@ -3864,7 +3586,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F314" s="21" t="b">
         <v>0</v>
@@ -3878,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F315" s="21" t="b">
         <v>0</v>
@@ -3892,7 +3614,7 @@
         <v>1</v>
       </c>
       <c r="E316" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F316" s="21" t="b">
         <v>0</v>
@@ -3906,7 +3628,7 @@
         <v>1</v>
       </c>
       <c r="E317" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F317" s="21" t="b">
         <v>0</v>
@@ -3920,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="E318" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F318" s="21" t="b">
         <v>0</v>
@@ -3934,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="E319" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F319" s="21" t="b">
         <v>0</v>
@@ -3948,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="E320" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F320" s="21" t="b">
         <v>0</v>
@@ -3956,13 +3678,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="22" t="s">
         <v>252</v>
-      </c>
-      <c r="C321" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E321" s="22" t="s">
-        <v>253</v>
       </c>
       <c r="F321" s="21" t="b">
         <v>0</v>
@@ -3970,7 +3692,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F322" s="21" t="b">
         <v>0</v>
@@ -4221,7 +3943,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
@@ -4238,7 +3960,7 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
@@ -4252,7 +3974,7 @@
         <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
fix(gams): ramping rate constraints ill defined.
Minor plotting fixes
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB8CBA-83FC-484F-9CFA-8B70BD21329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF517B6-C783-428F-A076-153C7A95E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,8 +1545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="C276" sqref="C276"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
         <v>46</v>
       </c>
       <c r="C59" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>86</v>
@@ -1952,7 +1952,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>63</v>
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="F169" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="H169" s="1" t="s">
         <v>175</v>
@@ -3340,7 +3340,7 @@
         <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(plot): enable plots to work with more than 50 zones and edit CPLEX options on configFile plot fixed: plot_zone_capacities, plot_energy_zone_fuel, plot_zone, plot_tech_cap, plot_power_flow_tracing_matrix
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goman\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF517B6-C783-428F-A076-153C7A95E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FE3E85-59FC-42EB-A632-459084D716C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="261">
   <si>
     <t>Default value</t>
   </si>
@@ -804,6 +804,21 @@
   </si>
   <si>
     <t>Price of Ammonia</t>
+  </si>
+  <si>
+    <t>CPLEX Accuracy</t>
+  </si>
+  <si>
+    <t>CPLEX Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Agressive</t>
   </si>
 </sst>
 </file>
@@ -964,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1080,6 +1095,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1545,36 +1563,36 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1584,20 +1602,20 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1607,21 +1625,21 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-    </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1630,7 +1648,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1639,7 +1657,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1648,7 +1666,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1657,7 +1675,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1666,7 +1684,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1675,7 +1693,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1684,7 +1702,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1693,7 +1711,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>177</v>
       </c>
@@ -1705,39 +1723,39 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="27"/>
     </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="32" t="s">
         <v>167</v>
       </c>
@@ -1749,7 +1767,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1764,7 +1782,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1778,7 +1796,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -1801,7 +1819,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -1813,24 +1831,44 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" s="40">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="28.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" ht="25.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" ht="51.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="32" t="s">
         <v>166</v>
       </c>
@@ -1842,7 +1880,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="33"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
@@ -1856,7 +1894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
@@ -1870,7 +1908,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
@@ -1884,7 +1922,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
@@ -1895,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
@@ -1906,7 +1944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -1917,19 +1955,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="32" t="s">
         <v>164</v>
       </c>
@@ -1941,10 +1979,10 @@
       <c r="G75" s="33"/>
       <c r="H75" s="33"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>41</v>
       </c>
@@ -1958,7 +1996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
@@ -1972,7 +2010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>123</v>
       </c>
@@ -1986,28 +2024,28 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
         <v>171</v>
       </c>
@@ -2019,7 +2057,7 @@
       <c r="G98" s="33"/>
       <c r="H98" s="33"/>
     </row>
-    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
@@ -2033,7 +2071,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -2047,7 +2085,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>174</v>
       </c>
@@ -2058,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="29" t="s">
         <v>172</v>
       </c>
@@ -2072,7 +2110,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="29" t="s">
         <v>173</v>
       </c>
@@ -2086,30 +2124,30 @@
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="32" t="s">
         <v>165</v>
       </c>
@@ -2121,7 +2159,7 @@
       <c r="G124" s="33"/>
       <c r="H124" s="33"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2136,7 +2174,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>199</v>
       </c>
@@ -2157,7 +2195,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2174,7 +2212,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2191,7 +2229,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
@@ -2205,7 +2243,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>40</v>
       </c>
@@ -2226,7 +2264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>48</v>
       </c>
@@ -2243,7 +2281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
@@ -2260,7 +2298,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>125</v>
       </c>
@@ -2277,7 +2315,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>124</v>
       </c>
@@ -2291,7 +2329,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>129</v>
       </c>
@@ -2305,7 +2343,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>196</v>
       </c>
@@ -2320,7 +2358,7 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>219</v>
       </c>
@@ -2334,7 +2372,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>224</v>
       </c>
@@ -2345,7 +2383,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>225</v>
       </c>
@@ -2356,7 +2394,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>226</v>
       </c>
@@ -2367,27 +2405,27 @@
         <v>223</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>216</v>
       </c>
@@ -2396,7 +2434,7 @@
       </c>
       <c r="C161" s="19"/>
     </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>215</v>
       </c>
@@ -2405,7 +2443,7 @@
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>209</v>
       </c>
@@ -2420,7 +2458,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -2434,8 +2472,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="32" t="s">
         <v>198</v>
       </c>
@@ -2447,7 +2485,7 @@
       <c r="G166" s="33"/>
       <c r="H166" s="33"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>121</v>
       </c>
@@ -2465,7 +2503,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>143</v>
       </c>
@@ -2483,7 +2521,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>135</v>
       </c>
@@ -2504,7 +2542,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>213</v>
       </c>
@@ -2525,7 +2563,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>217</v>
       </c>
@@ -2543,7 +2581,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>254</v>
       </c>
@@ -2561,15 +2599,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>119</v>
       </c>
@@ -2585,7 +2623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
@@ -2605,7 +2643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>61</v>
       </c>
@@ -2628,7 +2666,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>62</v>
       </c>
@@ -2648,7 +2686,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>120</v>
       </c>
@@ -2668,7 +2706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>126</v>
       </c>
@@ -2686,7 +2724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>127</v>
       </c>
@@ -2706,7 +2744,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>255</v>
       </c>
@@ -2724,22 +2762,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>144</v>
       </c>
@@ -2754,7 +2792,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>142</v>
       </c>
@@ -2769,7 +2807,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>145</v>
       </c>
@@ -2784,26 +2822,26 @@
         <v>147</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" spans="1:3" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="36" t="s">
         <v>168</v>
       </c>
@@ -2827,7 +2865,7 @@
       </c>
       <c r="H225" s="37"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>50</v>
       </c>
@@ -2850,8 +2888,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="41" t="s">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -2873,8 +2911,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="41"/>
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="42"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -2894,8 +2932,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="41"/>
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="42"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
       </c>
@@ -2915,8 +2953,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="41"/>
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="42"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
       </c>
@@ -2936,8 +2974,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="41"/>
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="42"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -2957,8 +2995,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="41"/>
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="42"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
@@ -2978,8 +3016,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="41"/>
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="42"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -2999,8 +3037,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="41"/>
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="42"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3020,8 +3058,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="41"/>
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="42"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3041,8 +3079,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="41"/>
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="42"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3062,8 +3100,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="41"/>
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="42"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3083,8 +3121,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="41"/>
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="42"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3104,8 +3142,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="41"/>
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="42"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3125,8 +3163,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="41"/>
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="42"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3146,8 +3184,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="41"/>
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="42"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3167,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3187,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3207,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="6" t="s">
         <v>19</v>
       </c>
@@ -3227,8 +3265,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="44" t="s">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="45" t="s">
         <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3250,8 +3288,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="44"/>
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="45"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
       </c>
@@ -3274,7 +3312,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3294,33 +3332,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="32" t="s">
         <v>72</v>
       </c>
@@ -3332,7 +3370,7 @@
       <c r="G274" s="33"/>
       <c r="H274" s="33"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3343,7 +3381,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>73</v>
       </c>
@@ -3357,7 +3395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>74</v>
       </c>
@@ -3371,7 +3409,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>76</v>
       </c>
@@ -3382,13 +3420,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="32" t="s">
         <v>169</v>
       </c>
@@ -3400,7 +3438,7 @@
       <c r="G298" s="33"/>
       <c r="H298" s="33"/>
     </row>
-    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>234</v>
       </c>
@@ -3413,7 +3451,7 @@
       <c r="G299" s="38"/>
       <c r="H299" s="38"/>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
         <v>90</v>
       </c>
@@ -3421,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B301" s="1" t="s">
         <v>91</v>
       </c>
@@ -3429,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B302" s="1" t="s">
         <v>95</v>
       </c>
@@ -3437,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B303" s="1" t="s">
         <v>97</v>
       </c>
@@ -3445,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="C304" s="13"/>
@@ -3455,7 +3493,7 @@
       <c r="G304" s="1"/>
       <c r="H304" s="1"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>235</v>
       </c>
@@ -3466,7 +3504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B306" s="22" t="s">
         <v>90</v>
       </c>
@@ -3480,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B307" s="22" t="s">
         <v>91</v>
       </c>
@@ -3494,7 +3532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B308" s="22" t="s">
         <v>92</v>
       </c>
@@ -3508,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B309" s="22" t="s">
         <v>93</v>
       </c>
@@ -3522,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B310" s="22" t="s">
         <v>94</v>
       </c>
@@ -3536,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B311" s="22" t="s">
         <v>95</v>
       </c>
@@ -3550,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B312" s="22" t="s">
         <v>96</v>
       </c>
@@ -3564,7 +3602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B313" s="22" t="s">
         <v>97</v>
       </c>
@@ -3578,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B314" s="22" t="s">
         <v>98</v>
       </c>
@@ -3592,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B315" s="22" t="s">
         <v>99</v>
       </c>
@@ -3606,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B316" s="22" t="s">
         <v>100</v>
       </c>
@@ -3620,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B317" s="22" t="s">
         <v>101</v>
       </c>
@@ -3634,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B318" s="22" t="s">
         <v>102</v>
       </c>
@@ -3648,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B319" s="22" t="s">
         <v>103</v>
       </c>
@@ -3662,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B320" s="22" t="s">
         <v>104</v>
       </c>
@@ -3676,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B321" s="22" t="s">
         <v>251</v>
       </c>
@@ -3690,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E322" s="22" t="s">
         <v>253</v>
       </c>
@@ -3698,12 +3736,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3816,7 +3854,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
@@ -3871,6 +3909,12 @@
           </x14:formula1>
           <xm:sqref>C101</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E809FE7-F26E-4691-BF39-5CA8B3998AB6}">
+          <x14:formula1>
+            <xm:f>Lists!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H40</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3880,22 +3924,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3914,8 +3959,11 @@
       <c r="F1" s="16" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3934,8 +3982,11 @@
       <c r="F2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3954,8 +4005,11 @@
       <c r="F3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -3969,7 +4023,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>130</v>
       </c>
@@ -3980,7 +4034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>133</v>
       </c>
@@ -4000,12 +4054,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="16" t="s">
         <v>105</v>
       </c>
@@ -4049,7 +4103,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>90</v>
       </c>
@@ -4096,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -4143,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>92</v>
       </c>
@@ -4190,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>93</v>
       </c>
@@ -4237,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
@@ -4284,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>95</v>
       </c>
@@ -4331,7 +4385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>96</v>
       </c>
@@ -4378,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>97</v>
       </c>
@@ -4425,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>98</v>
       </c>
@@ -4472,7 +4526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>99</v>
       </c>
@@ -4519,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>100</v>
       </c>
@@ -4566,7 +4620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>101</v>
       </c>
@@ -4613,7 +4667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
@@ -4660,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>103</v>
       </c>
@@ -4707,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
feat(gams): storage alert level included
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goman\Dispa-SET.git\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FE3E85-59FC-42EB-A632-459084D716C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B2DFDD-842B-45D1-ABB9-D05488D7A391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="263">
   <si>
     <t>Default value</t>
   </si>
@@ -819,6 +819,12 @@
   </si>
   <si>
     <t>Agressive</t>
+  </si>
+  <si>
+    <t>Reservoir Alert Levels</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/ReservoirAlertLevels.csv</t>
   </si>
 </sst>
 </file>
@@ -1564,23 +1570,23 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>221</v>
       </c>
@@ -1592,7 +1598,7 @@
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
     </row>
-    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1602,8 +1608,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="44" t="s">
         <v>56</v>
@@ -1615,7 +1621,7 @@
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1625,7 +1631,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
@@ -1639,7 +1645,7 @@
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1648,7 +1654,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1657,7 +1663,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1666,7 +1672,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1675,7 +1681,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1684,7 +1690,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1693,7 +1699,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1702,7 +1708,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1711,7 +1717,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>177</v>
       </c>
@@ -1723,39 +1729,39 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="27"/>
     </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>167</v>
       </c>
@@ -1767,7 +1773,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -1819,7 +1825,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>256</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="2" t="s">
         <v>257</v>
       </c>
@@ -1853,22 +1859,22 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:8" ht="28.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="25.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" ht="51.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="28.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="25.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="51.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>166</v>
       </c>
@@ -1880,7 +1886,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="33"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
@@ -1894,7 +1900,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
@@ -1922,7 +1928,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
@@ -1933,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -1955,19 +1961,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="32" t="s">
         <v>164</v>
       </c>
@@ -1979,10 +1985,10 @@
       <c r="G75" s="33"/>
       <c r="H75" s="33"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>41</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>123</v>
       </c>
@@ -2024,28 +2030,28 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
         <v>171</v>
       </c>
@@ -2057,7 +2063,7 @@
       <c r="G98" s="33"/>
       <c r="H98" s="33"/>
     </row>
-    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>174</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
         <v>172</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
         <v>173</v>
       </c>
@@ -2124,30 +2130,30 @@
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="32" t="s">
         <v>165</v>
       </c>
@@ -2159,7 +2165,7 @@
       <c r="G124" s="33"/>
       <c r="H124" s="33"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2174,7 +2180,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>199</v>
       </c>
@@ -2195,7 +2201,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>40</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>48</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>125</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>124</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>129</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>196</v>
       </c>
@@ -2358,7 +2364,7 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>219</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>224</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>225</v>
       </c>
@@ -2394,7 +2400,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>226</v>
       </c>
@@ -2405,27 +2411,37 @@
         <v>223</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C141" s="19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>216</v>
       </c>
@@ -2434,7 +2450,7 @@
       </c>
       <c r="C161" s="19"/>
     </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>215</v>
       </c>
@@ -2443,7 +2459,7 @@
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>209</v>
       </c>
@@ -2458,7 +2474,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -2472,8 +2488,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="32" t="s">
         <v>198</v>
       </c>
@@ -2485,7 +2501,7 @@
       <c r="G166" s="33"/>
       <c r="H166" s="33"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>121</v>
       </c>
@@ -2503,7 +2519,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>143</v>
       </c>
@@ -2521,7 +2537,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>135</v>
       </c>
@@ -2542,7 +2558,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>213</v>
       </c>
@@ -2563,7 +2579,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>217</v>
       </c>
@@ -2581,7 +2597,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>254</v>
       </c>
@@ -2599,15 +2615,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>119</v>
       </c>
@@ -2623,7 +2639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
@@ -2643,7 +2659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>61</v>
       </c>
@@ -2666,7 +2682,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>62</v>
       </c>
@@ -2686,7 +2702,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>120</v>
       </c>
@@ -2706,7 +2722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>126</v>
       </c>
@@ -2724,7 +2740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>127</v>
       </c>
@@ -2744,7 +2760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>255</v>
       </c>
@@ -2762,22 +2778,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>144</v>
       </c>
@@ -2792,7 +2808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>142</v>
       </c>
@@ -2807,7 +2823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>145</v>
       </c>
@@ -2822,26 +2838,26 @@
         <v>147</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" spans="1:3" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
         <v>168</v>
       </c>
@@ -2865,7 +2881,7 @@
       </c>
       <c r="H225" s="37"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>50</v>
       </c>
@@ -2888,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="42" t="s">
         <v>51</v>
       </c>
@@ -2911,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="42"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
@@ -2932,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="42"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
@@ -2953,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="42"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
@@ -2974,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="42"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -2995,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="42"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
@@ -3016,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="42"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
@@ -3037,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="42"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3058,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="42"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3079,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="42"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3100,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="42"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3121,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="42"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3142,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="42"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3163,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="42"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3184,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="42"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
@@ -3205,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3225,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3245,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
         <v>19</v>
       </c>
@@ -3265,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="45" t="s">
         <v>170</v>
       </c>
@@ -3288,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="45"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
@@ -3312,7 +3328,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3332,33 +3348,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="32" t="s">
         <v>72</v>
       </c>
@@ -3370,7 +3386,7 @@
       <c r="G274" s="33"/>
       <c r="H274" s="33"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3381,7 +3397,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>73</v>
       </c>
@@ -3395,7 +3411,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>74</v>
       </c>
@@ -3409,7 +3425,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>76</v>
       </c>
@@ -3420,13 +3436,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="32" t="s">
         <v>169</v>
       </c>
@@ -3438,7 +3454,7 @@
       <c r="G298" s="33"/>
       <c r="H298" s="33"/>
     </row>
-    <row r="299" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>234</v>
       </c>
@@ -3451,7 +3467,7 @@
       <c r="G299" s="38"/>
       <c r="H299" s="38"/>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
         <v>90</v>
       </c>
@@ -3459,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B301" s="1" t="s">
         <v>91</v>
       </c>
@@ -3467,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="1" t="s">
         <v>95</v>
       </c>
@@ -3475,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B303" s="1" t="s">
         <v>97</v>
       </c>
@@ -3483,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="C304" s="13"/>
@@ -3493,7 +3509,7 @@
       <c r="G304" s="1"/>
       <c r="H304" s="1"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>235</v>
       </c>
@@ -3504,7 +3520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B306" s="22" t="s">
         <v>90</v>
       </c>
@@ -3518,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B307" s="22" t="s">
         <v>91</v>
       </c>
@@ -3532,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B308" s="22" t="s">
         <v>92</v>
       </c>
@@ -3546,7 +3562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B309" s="22" t="s">
         <v>93</v>
       </c>
@@ -3560,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B310" s="22" t="s">
         <v>94</v>
       </c>
@@ -3574,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
         <v>95</v>
       </c>
@@ -3588,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B312" s="22" t="s">
         <v>96</v>
       </c>
@@ -3602,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B313" s="22" t="s">
         <v>97</v>
       </c>
@@ -3616,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B314" s="22" t="s">
         <v>98</v>
       </c>
@@ -3630,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B315" s="22" t="s">
         <v>99</v>
       </c>
@@ -3644,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B316" s="22" t="s">
         <v>100</v>
       </c>
@@ -3658,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B317" s="22" t="s">
         <v>101</v>
       </c>
@@ -3672,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B318" s="22" t="s">
         <v>102</v>
       </c>
@@ -3686,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B319" s="22" t="s">
         <v>103</v>
       </c>
@@ -3700,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B320" s="22" t="s">
         <v>104</v>
       </c>
@@ -3714,7 +3730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
         <v>251</v>
       </c>
@@ -3728,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
         <v>253</v>
       </c>
@@ -3736,12 +3752,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3930,17 +3946,17 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3963,7 +3979,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3986,7 +4002,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -4009,7 +4025,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -4023,7 +4039,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>130</v>
       </c>
@@ -4034,7 +4050,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>133</v>
       </c>
@@ -4054,12 +4070,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>105</v>
       </c>
@@ -4103,7 +4119,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>90</v>
       </c>
@@ -4150,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -4197,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>92</v>
       </c>
@@ -4244,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>93</v>
       </c>
@@ -4291,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
@@ -4338,7 +4354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>95</v>
       </c>
@@ -4385,7 +4401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>96</v>
       </c>
@@ -4432,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>97</v>
       </c>
@@ -4479,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>98</v>
       </c>
@@ -4526,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>99</v>
       </c>
@@ -4573,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>100</v>
       </c>
@@ -4620,7 +4636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>101</v>
       </c>
@@ -4667,7 +4683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
@@ -4714,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>103</v>
       </c>
@@ -4761,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
feat(spillage): cost of spillage can now be assigned for individual units
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B2DFDD-842B-45D1-ABB9-D05488D7A391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F0A452-8D75-456C-920E-0405609B95E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="264">
   <si>
     <t>Default value</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>tests/dummy_data/ReservoirAlertLevels.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/PriceOfSpillage.csv</t>
   </si>
 </sst>
 </file>
@@ -1569,8 +1572,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,7 +2815,12 @@
       <c r="A206" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C206" s="1"/>
+      <c r="B206" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C206" s="19" t="s">
+        <v>263</v>
+      </c>
       <c r="E206" s="25" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix(config): fixed the placement of CPLEX setting in the test configuration file
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTest.xlsx
+++ b/ConfigFiles/ConfigTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goman\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F0A452-8D75-456C-920E-0405609B95E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA963086-1C2C-4145-8BE6-F4897627A502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8250" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1572,24 +1572,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>221</v>
       </c>
@@ -1601,7 +1601,7 @@
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
     </row>
-    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1611,8 +1611,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="44" t="s">
         <v>56</v>
@@ -1624,7 +1624,7 @@
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1634,7 +1634,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1657,7 +1657,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1666,7 +1666,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1675,7 +1675,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1684,7 +1684,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1693,7 +1693,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1702,7 +1702,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1711,7 +1711,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1720,7 +1720,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>177</v>
       </c>
@@ -1732,39 +1732,39 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="27"/>
     </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="32" t="s">
         <v>167</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>256</v>
       </c>
@@ -1851,33 +1851,33 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="2" t="s">
+    <row r="40" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="B40" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="28.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="25.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="51.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="28.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" ht="25.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" ht="51.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="32" t="s">
         <v>166</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="33"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -1964,19 +1964,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="32" t="s">
         <v>164</v>
       </c>
@@ -1988,10 +1988,10 @@
       <c r="G75" s="33"/>
       <c r="H75" s="33"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>41</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>123</v>
       </c>
@@ -2033,28 +2033,28 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="32" t="s">
         <v>171</v>
       </c>
@@ -2066,7 +2066,7 @@
       <c r="G98" s="33"/>
       <c r="H98" s="33"/>
     </row>
-    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>174</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="29" t="s">
         <v>172</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="29" t="s">
         <v>173</v>
       </c>
@@ -2133,30 +2133,30 @@
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="32" t="s">
         <v>165</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="G124" s="33"/>
       <c r="H124" s="33"/>
     </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>199</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>40</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>48</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>125</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>124</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>129</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>196</v>
       </c>
@@ -2367,7 +2367,7 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>219</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>224</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>225</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>226</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>261</v>
       </c>
@@ -2425,26 +2425,26 @@
         <v>262</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>216</v>
       </c>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="C161" s="19"/>
     </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>215</v>
       </c>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>209</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -2491,8 +2491,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="32" t="s">
         <v>198</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="G166" s="33"/>
       <c r="H166" s="33"/>
     </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>121</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>143</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>135</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>213</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>217</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>254</v>
       </c>
@@ -2618,15 +2618,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>119</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>61</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>62</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>120</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>126</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>127</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>255</v>
       </c>
@@ -2781,22 +2781,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>144</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>142</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>145</v>
       </c>
@@ -2846,26 +2846,26 @@
         <v>147</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" spans="1:3" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="36" t="s">
         <v>168</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="H225" s="37"/>
     </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>50</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="42" t="s">
         <v>51</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="42"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="42"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="42"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="42"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="42"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="42"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="42"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="42"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
@@ -3103,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="42"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="42"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="42"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="42"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="42"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="42"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B244" s="6" t="s">
         <v>19</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="45" t="s">
         <v>170</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="45"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
@@ -3336,7 +3336,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3356,33 +3356,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="32" t="s">
         <v>72</v>
       </c>
@@ -3394,7 +3394,7 @@
       <c r="G274" s="33"/>
       <c r="H274" s="33"/>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>73</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>74</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>76</v>
       </c>
@@ -3444,13 +3444,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="32" t="s">
         <v>169</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="G298" s="33"/>
       <c r="H298" s="33"/>
     </row>
-    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>234</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="G299" s="38"/>
       <c r="H299" s="38"/>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
         <v>90</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B301" s="1" t="s">
         <v>91</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B302" s="1" t="s">
         <v>95</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B303" s="1" t="s">
         <v>97</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="C304" s="13"/>
@@ -3517,7 +3517,7 @@
       <c r="G304" s="1"/>
       <c r="H304" s="1"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>235</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B306" s="22" t="s">
         <v>90</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B307" s="22" t="s">
         <v>91</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B308" s="22" t="s">
         <v>92</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B309" s="22" t="s">
         <v>93</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B310" s="22" t="s">
         <v>94</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B311" s="22" t="s">
         <v>95</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B312" s="22" t="s">
         <v>96</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B313" s="22" t="s">
         <v>97</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B314" s="22" t="s">
         <v>98</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B315" s="22" t="s">
         <v>99</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B316" s="22" t="s">
         <v>100</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B317" s="22" t="s">
         <v>101</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B318" s="22" t="s">
         <v>102</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B319" s="22" t="s">
         <v>103</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B320" s="22" t="s">
         <v>104</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B321" s="22" t="s">
         <v>251</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E322" s="22" t="s">
         <v>253</v>
       </c>
@@ -3760,12 +3760,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3937,7 +3937,7 @@
           <x14:formula1>
             <xm:f>Lists!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H40</xm:sqref>
+          <xm:sqref>C40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3954,17 +3954,17 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>130</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>133</v>
       </c>
@@ -4078,12 +4078,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="16" t="s">
         <v>105</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>90</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>92</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>93</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>95</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>96</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>97</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>98</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>99</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>100</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>101</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>103</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>104</v>
       </c>

</xml_diff>